<commit_message>
Pipeline working with 2 partitions
</commit_message>
<xml_diff>
--- a/image_preprocessing/two_vertex/accuracy_degradation/virtual/virtual_image_classification.xlsx
+++ b/image_preprocessing/two_vertex/accuracy_degradation/virtual/virtual_image_classification.xlsx
@@ -11,6 +11,12 @@
     <sheet name="Planner Configuration" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Planner Config Run Results" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Planner Config Run Results(Raw)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Planner Config Run Results1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Planner Config Run Results(Raw)1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Planner Config Run Results2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Planner Config Run Results(Raw)2" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Planner Config Run Results3" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Planner Config Run Results(Raw)3" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -491,6 +497,108 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mu (qps)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cv</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t># requests</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Latency Constraint (ms)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Planner</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estimated Latency (ms)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Latency (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>SimulatedAnnealing</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>71.74977540969849</v>
+      </c>
+      <c r="H2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">[71.19626086205244, 53.83584462106228, 53.726743906736374, 87.87885122001171, 89.86424840986729, 100.7017707452178, 97.32230845838785, 92.76306163519621, 83.56313034892082, 82.43606146425009, 70.7133300602436, 66.46362878382206, 57.027410715818405, 55.66141568124294, 47.34424781054258, 37.71490138024092, 34.99657940119505, 35.855614580214024, 35.66902130842209, 35.43929196894169, 35.65720468759537, 35.12845002114773, 35.37626937031746, 36.50414291769266, 36.025152541697025, 36.3682871684432, 36.237794905900955, 36.56620718538761, 36.592758260667324, 36.41228936612606, 37.10188530385494, 37.69438061863184, 37.29941323399544, 37.87158150225878, 37.4835254624486, 38.497380912303925, 39.041658863425255, 40.375289507210255, 37.48147655278444, 36.68116871267557, 45.83280999213457, 37.28077840059996, 36.69544402509928, 36.85314487665892, 35.93470063060522, 36.68118640780449, 38.06325886398554, 36.26388777047396, 37.44545113295317, 39.44122605025768, 38.609485141932964, 37.45115268975496, 36.123394034802914, 39.61454425007105, 37.58765570819378, 36.56421694904566, 37.54386678338051, 38.26395235955715, 38.40229753404856, 36.19476407766342, 36.45095881074667, 38.38901035487652, 37.769281305372715, 37.25282661616802, 38.66354189813137, 37.132744677364826, 35.81701312214136, 37.487978115677834, 38.68701495230198, 37.12593298405409, 37.17817086726427, 49.0984795615077, 43.877048417925835, 42.00862254947424, 37.64437232166529, 35.8939953148365, 43.83176937699318, 35.652381367981434, 35.75817681849003, 42.039782740175724, 41.70648381114006, 37.564467638731, 38.79945818334818, 37.05355525016785, 42.13887732475996, 39.98785652220249, 37.148818373680115, 58.27153101563454, 49.05242193490267, 56.29831086844206, 47.30463773012161, 45.67081108689308, 36.99105139821768, 42.02073160558939, 36.59416455775499, 35.14567390084267, 35.47929506748915, 41.2922827526927, 42.12956316769123, 38.03002741187811, 43.36991533637047, 37.713500671088696, 43.04195940494537, 36.76780965179205, 34.96381174772978, 40.834736078977585, 41.64065420627594, 36.020961590111256, 38.30109443515539, 37.205640226602554, 43.34799014031887, 53.74681483954191, 41.501544415950775, 42.549134232103825, 43.828366324305534, 37.21348010003567, 37.370155565440655, 38.07428665459156, 40.40966276079416, 36.16756573319435, 37.445299327373505, 39.06218055635691, 34.78201851248741, 41.12765472382307, 38.29489089548588, 41.57729260623455, 36.06681618839502, 38.86173851788044, 38.575840182602406, 42.00619272887707, 37.96389512717724, 36.87186259776354, 37.163606844842434, 37.37636283040047, 35.334150306880474, 36.09968721866608, 37.51891106367111, 38.05918339639902, 37.88990620523691, 36.49393655359745, 37.01736684888601, 37.165150977671146, 34.19751301407814, 34.517234191298485, 37.61689271777868, 37.09247335791588, 35.57271417230368, 36.71915456652641, 38.46208844333887, 37.85974811762571, 38.39803021401167, 37.78599388897419, 38.23126945644617, 38.06385491043329, 37.2786121442914, 40.029849857091904, 159.63221061974764, 155.21219931542873, 164.98726047575474, 197.19740096479654, 196.65683060884476, 196.94141298532486, 186.7842571809888, 183.9900715276599, 174.5396088808775, 171.9741178676486, 162.4957164749503, 158.54901913553476, 149.2896368727088, 146.06968965381384, 136.2088844180107, 132.72181060165167, 123.93420469015837, 120.07794063538313, 110.86173076182604, 107.75757301598787, 99.10092316567898, 92.09503140300512, 83.98514334112406, 82.27011933922768, 72.7001540362835, 64.13253210484982, 52.16207820922136, 54.980711080133915, 46.75071872770786, 35.65651085227728, 39.54776003956795, 36.2677751109004, 37.24703658372164, 37.25333884358406, 42.572686448693275, 36.763074807822704, 37.1357835829258, 36.85086499899626, 37.253872491419315, 46.10844235867262, 52.26296093314886, 43.12241170555353, 45.66822573542595, 41.68926179409027, 34.910717979073524, 38.30025810748339, 41.998605243861675, 38.45333494246006, 42.26190783083439, 42.063808999955654, 39.88010808825493, 38.10684476047754, 37.626802921295166, 37.36442048102617, 37.95709181576967, 36.534132435917854, 37.459198385477066, 37.53641992807388, 38.47127500921488, 38.76170702278614, 41.696904227137566, 35.83624493330717, 36.917020566761494, 38.22627943009138, 38.17414026707411, 36.245064809918404, 37.27302327752113, 43.029117397964, 37.400356493890285, 41.156526654958725, 37.141818553209305, 37.762513384222984, 37.98471391201019, 36.305985413491726, 34.22870393842459, 39.70205783843994, 35.51560267806053, 36.876341328024864, 37.752844393253326, 39.33858033269644, 36.584436893463135, 36.622279323637486, 36.51944827288389, 37.97548357397318, 42.22546238452196, 36.749512888491154, 36.508181132376194, 42.160267010331154, 39.621563628315926, 36.806149408221245, 38.06161507964134, 41.83910973370075, 41.34988505393267, 36.1105240881443, 34.95232481509447, 38.31692412495613, 36.63013502955437, 36.291792057454586, 43.265391141176224, 38.29616401344538, 42.28692315518856, 35.592103376984596, 35.490550100803375, 41.313331574201584, 42.10118297487497, 38.109940476715565, 36.785067059099674, 35.031883046031, 35.54639592766762, 38.43577019870281, 38.691761903464794, 35.84742918610573, 37.73929737508297, 38.225301541388035, 35.90867388993502, 35.95950733870268, 40.11133499443531, 41.71371925622225, 36.01210657507181, 35.45790258795023, 41.92580655217171, 40.24345055222511, 34.6560925245285, 34.43603217601776, 34.28762033581734, 32.90469292551279, 34.86185893416405, 40.95116630196571, 42.47467219829559, 35.79174540936947, 38.460781797766685, 34.74606666713953, 35.07695533335209, 38.692585192620754, 42.69242472946644, 36.91478259861469, 35.822669044137, 41.99554957449436, 42.15024411678314, 37.56186459213495, 34.24971643835306, 36.46868094801903, 41.20365530252457, 34.63221155107021, 35.62360908836126, 38.807036355137825, 37.879398092627525, 38.1099684163928, 34.89955514669418, 36.01421322673559, 35.704570822417736, 34.50253140181303, 35.21375823765993, 35.471624694764614, 35.82638129591942, 37.354529835283756, 38.745203986763954, 35.420975647866726, 34.120844677090645, 37.81487047672272, 42.422705329954624, 46.52199428528547, 37.845682352781296, 39.4631689414382, 35.79591866582632, 35.49306560307741, 35.55695619434118, 35.37019435316324, 35.082852467894554, 34.09785497933626, 35.840267315506935, 36.890177987515926, 35.119946114718914, 35.43734084814787, 35.46837158501148, 37.001876160502434, 35.791654139757156, 36.81761585175991, 35.44296510517597, 36.908650770783424, 37.76658046990633, 33.580622635781765, 35.75138375163078, 36.113872192800045, 36.096871830523014, 34.76342000067234, 35.15211120247841, 37.324427627027035, 34.74566526710987, 35.1015804335475, 35.037221387028694, 35.86150147020817, 34.590196795761585, 35.49101483076811, 34.90801993757486, 36.02848667651415, 34.87381897866726, 34.64655112475157, 35.76072305440903, 40.06058629602194, 43.01254916936159, 36.17761563509703, 37.26201597601175, 41.10846761614084, 41.358557529747486, 37.475003860890865, 35.28604190796614, 36.81463282555342, 35.179056227207184, 36.074044182896614, 35.55537760257721, 35.525307059288025, 35.900019109249115, 37.248422391712666, 37.76239324361086, 38.674622774124146, 36.96001227945089, 40.28021264821291, 43.562243692576885, 46.063278801739216, 42.495316825807095, 39.37340993434191, 38.39895315468311, 34.30734854191542, 39.696551859378815, 34.51045695692301, 37.31204476207495, 36.28513868898153, 51.771736703813076, 50.796995870769024, 45.22197972983122, 44.22342777252197, 34.86199863255024, 34.71926134079695, 40.83217680454254, 34.9437240511179, 36.871955730021, 37.44172118604183, 38.788024336099625, 37.71524876356125, 37.395927123725414, 39.438449777662754, 39.07220717519522, 36.97662707418203, 35.74089799076319, 36.75997722893953, 38.634875789284706, 39.73689489066601, 36.308943293988705, 36.11416835337877, 43.3028768748045, 35.20128130912781, 36.75430174916983, 38.640812039375305, 38.62056881189346, 36.38043347746134, 37.132805213332176, 38.12461532652378, 39.107104763388634, 37.11564373224974, 36.048101261258125, 37.98387758433819, 43.16793009638786, 35.61387583613396, 37.346117198467255, 37.570903077721596, 36.65099199861288, 37.482718005776405, 40.224721655249596, 35.929566249251366, 41.559359058737755, 37.72305138409138, 35.95092799514532, 34.44261848926544, 36.88791859894991, 38.435750640928745, 38.22921309620142, 36.97605710476637, 42.16202720999718, 40.73500633239746, 36.006429232656956, 35.55728495121002, 42.18954127281904, 35.48540361225605, 34.67062767595053, 38.51523995399475, 43.60936675220728, 54.073539562523365, 44.706517830491066, 51.67159251868725, 42.63599589467049, 42.08988510072231, 35.74291430413723, 33.82462356239557, 47.2585242241621, 58.03511571139097, 50.59467256069183, 44.39791105687618, 40.27762170881033, 36.24750953167677, 33.122170716524124, 41.50058329105377, 41.46811366081238, 35.62487289309502, 38.957299664616585, 35.686079412698746, 36.83885373175144, 38.394139148294926, 37.98261843621731, 35.38983874022961, 35.483685322105885, 37.81993966549635, 35.91804392635822, 33.26927591115236, 34.60578341037035, 33.420562744140625, 37.323023192584515, 43.917933478951454, 39.522482082247734, 38.54896780103445, 39.25168886780739, 39.67469185590744, 37.27961145341396, 35.853431560099125, 37.324078381061554, 34.76348519325256, 33.66201929748058, 34.213028848171234, 37.16502618044615, 38.612968288362026, 37.584430538117886, 34.83154997229576, 35.78856587409973, 38.22620585560799, 35.37219297140837, 35.50557978451252, 37.407892756164074, 35.69870814681053, 35.29789485037327, 36.29669360816479, 39.50893133878708, 42.52417013049126, 42.519266717135906, 36.31173074245453, 41.94491356611252, 35.2848581969738, 45.304407365620136, 43.17473154515028, 37.33710199594498, 37.16082312166691, 43.02193969488144, 43.82953140884638, 35.13269033282995, 40.00616632401943, 34.95587408542633, 37.21640910953283, 35.80812364816666, 39.204840548336506, 36.5750202909112, 43.20777766406536, 37.27591410279274, 38.06070517748594, 36.68599482625723, 41.29741061478853, 36.4723838865757, 38.24254125356674, 38.01688924431801, 38.28977793455124, 38.907441310584545, 44.92757096886635, 36.93388029932976, 37.59815637022257, 37.134687416255474, 37.7982072532177, 39.50108680874109, 39.898831397295, 37.064360454678535, 36.24632861465216, 37.625815719366074, 36.77147347480059, 36.63587477058172, 37.809886038303375, 36.03960946202278, 38.485671393573284, 36.09944507479668, 37.71756403148174, 37.23579924553633, 38.65433856844902, 38.29766344279051, 37.61082887649536, 37.37093694508076, 41.30847193300724, 37.673477083444595, 37.68903575837612, 38.695527240633965, 37.97900676727295, 36.292788572609425, 39.527726359665394, 39.805565029382706, 37.03304287046194, 38.29011507332325, 42.22335293889046, 36.442384123802185, 42.18550864607096, 38.19529991596937, 36.70965600758791, 36.54809668660164, 37.382726557552814, 37.698905915021896, 37.956093437969685, 37.98626735806465, 39.02081772685051, 36.68009303510189, 42.02262591570616, 36.43766511231661, 36.74912918359041, 38.85413147509098, 37.1086448431015, 35.735324025154114, 52.26222425699234, 41.10250249505043, 45.39492912590504, 37.56456729024649, 35.126810893416405, 37.36481070518494, 35.809499211609364, 35.59267148375511, 41.97975527495146, 43.450730852782726, 36.12141311168671, 36.9534632191062, 38.038874976336956, 37.60217875242233, 39.06746208667755, 38.585688918828964, 36.7404455319047, 41.824969463050365, 44.2817248404026, 38.255984894931316, 36.452061496675014, 39.389765821397305, 38.88324927538633, 40.3131740167737, 37.22073417156935, 36.223435774445534, 42.576017789542675, 38.573737256228924, 37.35463786870241, 39.50715623795986, 36.119913682341576, 39.54645060002804, 36.14696301519871, 33.54492038488388, 36.92332096397877, 36.9244571775198, 34.40506011247635, 38.08658104389906, 42.85857919603586, 47.33745288103819, 42.90123004466295, 42.212885804474354, 40.504224598407745, 35.93237418681383, 37.59714588522911, 38.31667359918356, 41.41350742429495, 38.57835568487644, 36.59821953624487, 36.77817061543465, 35.00528912991285, 36.8202431127429, 42.493583634495735, 46.440799720585346, 42.125084437429905, 45.63078656792641, 48.828029073774815, 55.188694037497044, 47.2126929089427, 52.93069779872894, 43.60622074455023, 41.331833228468895, 34.3636991456151, 34.61452107876539, 38.05059567093849, 34.018732607364655, 33.90577342361212, 38.9015544205904, 39.44409731775522, 37.13296726346016, 35.48730444163084, 35.998206585645676, 37.45828103274107, 38.1379434838891, 40.81082344055176, 35.05844157189131, 36.88829019665718, 42.82535891979933, 33.75612664967775, 34.03483238071203, 36.62837669253349, 34.41338613629341, 36.79957985877991, 36.07590589672327, 37.418073043227196, 37.27790713310242, 35.685512237250805, 35.059104673564434, 35.31491197645664, 35.96250340342522, 34.93022546172142, 35.34037992358208, 36.03485692292452, 37.018897011876106, 35.60016304254532, 34.157268702983856, 34.15204677730799, 36.37663088738918, 35.63962131738663, 33.796329982578754, 36.249895580112934, 43.52769162505865, 35.779441706836224, 38.59769459813833, 34.84795056283474, 34.93901900947094, 35.05744785070419, 34.340254962444305, 35.696218721568584, 36.836146377027035, 36.660089157521725, 35.93695256859064, 36.73346992582083, 33.93176756799221, 35.36988142877817, 35.05843784660101, 35.207889042794704, 35.034794360399246, 36.057510413229465, 37.10203152149916, 34.03210919350386, 35.62115132808685, 37.21269592642784, 38.956113159656525, 35.4792345315218, 37.393976002931595, 34.645975567400455, 36.47816460579634, 34.2451948672533, 37.74874843657017, 34.217873588204384, 35.97485087811947, 34.06805917620659, 36.33717820048332, 34.265125170350075, 35.59181001037359, 35.184127278625965, 35.24505626410246, 35.55886447429657, 35.509693436324596, 39.710075594484806, 36.27954889088869, 33.833395689725876, 39.257884956896305, 41.35885089635849, 37.03787177801132, 34.714801236987114, 41.94491729140282, 35.99076997488737, 36.737848073244095, 36.69257182627916, 39.508212357759476, 37.96986769884825, 36.56597249209881, 38.693285547196865, 37.054901011288166, 35.36024037748575, 43.26936602592468, 41.54466465115547, 35.87396163493395, 36.77176032215357, 41.806722059845924, 37.14143857359886, 36.62044554948807, 35.38321703672409, 37.48895134776831, 38.426775485277176, 37.934317253530025, 35.77842004597187, 38.901050575077534, 42.40495339035988, 36.782676354050636, 35.969856195151806, 36.43512353301048, 42.61448234319687, 36.935520358383656, 36.16784047335386, 35.82557290792465, 41.724152863025665, 39.96630758047104, 41.364152915775776, 42.545489966869354, 35.6178218498826, 37.016622722148895, 36.68913245201111, 33.13138708472252, 36.33855190128088, 42.51034464687109, 37.23040781915188, 36.01920325309038, 41.78520292043686, 34.957196563482285, 35.96929553896189, 39.26978167146444, 37.07690443843603, 42.41463355720043, 41.80454555898905, 38.56608830392361, 34.636128693819046, 37.60728519409895, 42.617606930434704, 34.740278497338295, 35.18651891499758, 36.56234033405781, 35.02160310745239, 38.41320797801018, 42.11249575018883, 40.52560403943062, 36.07206977903843, 33.41870196163654, 34.503635950386524, 37.46406454592943, 38.42586651444435, 36.90887149423361, 37.21239324659109, 35.21245252341032, 125.3259927034378, 115.50049856305122, 123.30078147351742, 54.32948749512434, 57.561177760362625, 110.08634325116873, 114.63219858705997, 125.01987814903259, 122.85829335451126, 130.15091326087713, 129.97567933052778, 135.77578403055668, 135.5672711506486, 145.0521359220147, 139.20817896723747, 130.6266924366355, 120.7598689943552, 121.10974546521902, 111.60094942897558, 103.55710424482822, 92.01586898416281, 93.5267498716712, 85.44637355953455, 75.50508435815573, 66.45249761641026, 66.33644551038742, 56.84288498014212, 47.69784398376942, 45.58592848479748, 38.37252873927355, 35.56491155177355, 35.16445402055979, 35.0843071937561, 37.46672626584768, 35.27336847037077, 38.08835335075855, 36.09554283320904, 38.07361610233784, 35.49367468804121, 37.92231623083353, 37.60961256921291, 38.30819483846426, 36.59612964838743, 36.95007413625717, 37.2059466317296, 37.28946205228567, 36.439075134694576, 37.52898704260588, 37.00567502528429, 42.109708301723, 43.366449885070324, 38.351490162312984, 38.93506992608309, 38.22052199393511, 36.170074716210365, 41.9505313038826, 36.026882007718086, 42.30678919702768, 41.505275294184685, 37.41210699081421, 37.319958209991455, 42.29090828448534, 36.25922184437513, 36.23981587588787, 36.47434897720814, 35.45787278562784, 36.441922187805176, 35.2134183049202, 35.63133254647255, 35.370877012610435, 35.87395139038563, 35.93145031481981, 36.50035709142685, 38.276457227766514, 40.04340711981058, 35.93120630830526, 36.20758280158043, 37.85734158009291, 35.64911521971226, 36.84387821704149, 36.149694584310055, 38.38451951742172, 35.31610034406185, 36.42341494560242, 36.89505439251661, 41.967750526964664, 42.35691297799349, 41.10881872475147, 35.78812815248966, 34.89988762885332, 36.29710804671049, 36.09585762023926, 36.89730539917946, 46.19857110083103, 37.48730383813381, 36.81358601897955, 35.72906833142042, 38.91308419406414, 37.149581126868725, 36.691537126898766, 36.89019754528999, 36.63183469325304, 37.4700715765357, 41.15635994821787, 35.2022061124444, 34.97875761240721, 37.42937184870243, 45.54392769932747, 42.481991462409496, 40.24604521691799, 45.1529435813427, 51.29162408411503, 45.4329252243042, 45.83857022225857, 38.90876192599535, 36.48456837981939, 36.42519935965538, 39.53645005822182, 41.65825620293617, 35.03946214914322, 38.12790382653475, 45.63296493142843, 35.99709365516901, 38.37261628359556, 36.338488571345806, 35.352365113794804, 36.85149922966957, 40.49627669155598, 36.53120808303356, 37.16546483337879, 37.64533717185259, 41.364152915775776, 46.56110983341932, 42.848533019423485, 39.56564702093601, 42.4675140529871, 55.96208665519953, 50.29821116477251, 57.30482377111912, 47.29837458580732, 45.06813641637564, 36.91338934004307, 42.76329278945923, 33.838799223303795, 38.33595849573612, 42.85619594156742, 43.602997437119484, 38.000826723873615, 42.2863382846117, 38.84292207658291, 40.93936737626791, 35.78411415219307, 36.47440392524004, 41.428654454648495, 36.37317568063736, 37.0053481310606, 38.75627275556326, 42.65782609581947, 33.75947941094637, 36.39250062406063, 42.26860124617815, 38.181803189218044, 40.82550574094057, 34.800986759364605, 35.273983143270016, 38.16402703523636, 33.57973415404558, 38.98631688207388, 38.87971676886082, 36.56172938644886, 44.06912624835968, 36.47105861455202, 41.436824947595596, 35.85725277662277, 39.5232317969203, 41.30303580313921, 33.96639134734869, 34.51686818152666, 37.62374632060528, 36.00689955055714, 34.5626100897789, 35.376252606511116, 35.74369382113218, 33.00464991480112, 36.83995269238949, 37.02223859727383, 38.31265401095152, 40.624755434691906, 38.091239519417286, 36.29439789801836, 53.14512085169554, 53.337824530899525, 46.70126177370548, 46.55225295573473, 37.32358384877443, 34.94131099432707, 35.792834125459194, 33.20609591901302, 35.142334178090096, 40.8161710947752, 34.61280558258295, 34.83049850910902, 37.69388608634472, 37.04733680933714, 41.21451359242201, 36.954786628484726, 34.947749227285385, 36.361881531775, 36.667841486632824, 37.008718587458134, 34.529694356024265, 35.760543309152126, 34.60194915533066, 35.736678168177605, 37.904768250882626, 37.3683450743556, 36.184052005410194, 38.07029593735933, 36.640155129134655, 40.17477575689554, 36.14610340446234, 36.92296799272299, 35.30348464846611, 36.71331610530615, 36.82437539100647, 36.62916272878647, 35.65949946641922, 34.79453921318054, 37.25494537502527, 40.209769271314144, 36.393883638083935, 37.06302586942911, 35.0011233240366, 36.75063140690327, 35.145836882293224, 35.13193130493164, 35.36425344645977, 34.70304794609547, 35.32882779836655, 34.61383190006018, 34.73210334777832, 37.6586252823472, 38.26074115931988, 42.69555676728487, 35.627988167107105, 38.07509131729603, 36.58259101212025, 35.14932468533516, 35.0151602178812, 34.571913070976734, 34.697781316936016, 34.201713278889656, 35.774657502770424, 38.32804411649704, 36.814586259424686, 38.4822404012084, 40.559615008533, 40.70277791470289, 35.21622996777296, 35.61492636799812, 35.60175746679306, 36.80517431348562, 35.44538002461195, 36.10624838620424, 33.69074501097202, 36.510796286165714, 36.28192096948624, 35.4222459718585, 35.25948338210583, 35.388209857046604, 36.552305333316326, 37.664879113435745, 45.31202185899019, 38.81861548870802, 38.961971178650856, 36.03014163672924, 44.760908000171185, 35.375588573515415, 36.954279989004135, 34.45578273385763, 36.36107034981251, 34.64668896049261, 36.1400730907917, 35.64652521163225, 37.53496892750263, 35.947746597230434, 38.34129590541124, 40.387408807873726, 36.4331379532814, 36.478035151958466, 37.1054382994771, 36.31290886551142, 43.16037707030773, 42.37080831080675, 35.763864405453205, 36.79293300956488, 34.463643096387386, 32.46396780014038, 36.77976876497269, 35.55099945515394, 35.729280672967434, 38.91362063586712, 38.82864490151405, 48.655321821570396, 44.71513442695141, 40.01208860427141, 36.529759876430035, 39.59065303206444, 42.41874162107706, 41.10561404377222, 44.55673415213823, 45.257662422955036, 38.36826700717211, 38.39896712452173, 37.1626578271389, 34.81147438287735, 33.90256408601999, 33.19716267287731, 35.8113469555974, 36.78743913769722, 38.05603738874197, 37.67446894198656, 35.77442932873964, 36.55351419001818, 37.47746720910072, 37.858772091567516, 37.255095317959785, 36.824363283813, 37.269908003509045, 44.816928915679455, 39.985012263059616, 40.655212476849556, 33.61667226999998, 33.82244519889355, 35.60849279165268, 37.14238200336695, 38.74492924660444, 34.99358706176281, 40.17172008752823, 43.56908146291971, 37.475899793207645, 36.70184686779976, 34.64697301387787, 38.58675993978977, 40.3723269701004, 40.01255985349417, 33.27310550957918, 35.95244511961937, 37.968672811985016, 37.80606389045715, 35.289423540234566, 37.97186352312565, 38.38217817246914, 43.278492987155914, 37.139883264899254, 41.923568584024906, 42.20118187367916, 36.79581172764301, 35.359726287424564, 34.19500216841698, 34.664141945540905, 42.25037433207035, 37.95481380075216, 36.81651595979929, 36.248802207410336, 36.19084693491459, 36.05938050895929, 39.36467971652746, 45.11238634586334, 37.05435525625944, 42.237091809511185, 41.28793440759182, 40.42935650795698, 34.286764450371265, 34.94017664343119, 37.886480800807476, 34.098382107913494, 35.672285594046116, 36.038774996995926, 37.58759889751673, 37.4265480786562, 35.783265717327595, 38.2656492292881, 37.332803942263126, 35.874114371836185, 39.56513665616512, 38.046110421419144, 37.00072877109051, 36.08912229537964, 36.99015360325575, 36.89893428236246, 33.77943020313978, 38.66421617567539, 45.19792087376118, 38.27401716262102, 42.250605300068855, 35.24000197649002, 36.57520655542612, 35.88698524981737, 35.5070186778903, 35.48425901681185, 36.28216404467821, 37.670488469302654, 36.96964215487242, 39.383876137435436, 35.507166758179665, 36.11288592219353, 33.811746165156364, 35.20437702536583, 35.837999545037746, 35.08543502539396, 37.769123911857605, 35.37297993898392, 34.451414830982685, 34.939683973789215, 38.29642478376627, 36.14318277686834, 36.1246969550848, 34.683894366025925, 36.37245297431946, 36.017123609781265, 34.93793681263924, 35.22249311208725, 34.529777243733406, 34.638699144124985, 34.341176971793175, 34.56487134099007, 35.80736927688122, 35.47116182744503, 35.73391679674387, 33.66528917104006, 37.35595755279064, 41.61881376057863, 34.74465012550354, 42.598952539265156, 33.91536325216293, 34.71382800489664, 35.57256981730461, 33.27575698494911, 35.016695968806744, 35.283044911921024, 35.10902263224125, 35.11261474341154, 34.28015485405922, 34.620871767401695, 34.18011590838432, 34.41482875496149, 36.5305170416832, 36.638098768889904, 34.937476739287376, 42.07298252731562, 34.47201196104288, 37.32828237116337, 35.58548353612423, 34.40820146352053, 35.0136561319232, 34.45357549935579, 36.611597053706646, 37.06459607928991, 34.22558307647705, 38.82941883057356, 33.73836167156696, 38.2432397454977, 35.386442206799984, 36.447674967348576, 40.89551791548729, 37.00882848352194, 35.666706040501595, 36.89052443951368, 57.78123904019594, 52.46326141059399, 57.51356389373541, 48.221650533378124, 41.68306477367878, 38.44098560512066, 43.38858462870121, 34.44644436240196, 36.08131129294634, 38.53773046284914, 34.93900131434202, 38.309005089104176, 34.823354333639145, 36.52848117053509, 36.093960516154766, 37.42912597954273, 36.431122571229935, 37.336490117013454, 37.02226001769304, 43.13903674483299, 38.29255234450102, 37.63711545616388, 36.736397072672844, 41.82223416864872, 39.02404382824898, 42.12002083659172, 36.061445251107216, 35.58086045086384, 41.482687927782536, 37.12649364024401, 44.72101107239723, 47.264523804187775, 38.00818044692278, 43.23899187147617, 35.43110843747854, 34.40660238265991, 39.702631533145905, 39.74868729710579, 41.80164635181427, 37.34091389924288, 43.020812794566154, 38.26106619089842, 36.20926942676306, 36.22604068368673, 35.19026190042496, 39.90630805492401, 45.238422229886055, 37.996118888258934, 39.83539901673794, 36.682612262666225, 34.932371228933334, 36.71743255108595, 37.568630650639534, 37.978364154696465, 44.79534458369017, 36.817301996052265, 36.22355218976736, 42.29349456727505, 39.78400118649006, 37.467959336936474, 34.162746742367744, 36.50854993611574, 39.79197982698679, 36.5532711148262, 42.85028576850891, 42.81739052385092, 34.264808520674706, 36.23934183269739, 37.954255007207394, 33.328695222735405, 36.14073619246483, 36.45922988653183, 42.34419111162424, 41.454244405031204, 37.58798073977232, 35.098196007311344, 37.428854033350945, 33.55663549154997, 36.11480072140694, 40.01946561038494, 42.47239604592323, 39.34153262525797, 43.91270875930786, 38.358245976269245, 35.17946880310774, 37.53100335597992, 35.53752414882183, 35.28391197323799, 37.71273884922266, 38.841607980430126, 36.61662898957729, 38.3905740454793, 33.3338575437665, 40.06416443735361, 42.93301701545715, 34.50103383511305, 38.73669542372227, 36.56137827783823, 35.371760837733746, 41.49603843688965, 37.896327674388885, 33.184739761054516, 36.32182814180851, 35.386242903769016, 35.84135323762894, 42.22528915852308, 35.04228871315718, 34.89919472485781, 40.80378916114569, 34.829641692340374, 35.084000788629055, 38.376771844923496, 33.41770637780428, 38.39362319558859, 36.67331766337156, 35.58555990457535, 36.9094405323267, 35.621956922113895, 35.06972920149565, 38.03683631122112, 36.75180394202471, 35.902708768844604, 36.73459682613611, 35.04395764321089, 40.45094735920429, 38.80474716424942, 46.728700399398804, 38.16178906708956, 45.29234487563372, 42.48871095478535, 36.701226606965065, 38.6665528640151, 36.36300377547741, 36.77331283688545, 35.94949655234814, 36.67100518941879, 35.48076096922159, 35.87270062416792, 34.06026493757963, 35.48954240977764, 34.67377554625273, 35.48920154571533, 36.477611400187016, 40.8006701618433, 34.55780819058418, 34.280662424862385, 33.44324789941311, 33.85145589709282, 34.086788073182106, 35.06392054259777, 34.41959712654352, 34.34259723871946, 34.138478338718414, 33.81418902426958, 34.85347889363766, 33.912341110408306, 34.36987940222025, 34.97194033116102, 35.16368940472603, 34.170642495155334, 34.48630217462778, 41.34697746485472, 34.85167399048805, 36.096266470849514, 33.92664063721895, 34.51675269752741, 33.1652881577611, 34.319860860705376, 35.054261796176434, 34.595719538629055, 34.54617690294981, 35.67090816795826, 35.53342819213867, 36.71275358647108, 36.70998103916645, 40.62126111239195, 35.45059449970722, 36.84540465474129, 35.20573955029249, 37.67464496195316, 36.48616559803486, 44.709376990795135, 42.38531831651926, 36.45006846636534, 35.59308126568794, 35.15467792749405, 35.46625282615423, 34.26831867545843, 35.85456870496273, 32.8677948564291, 33.520533703267574, 35.47987062484026, 32.78172202408314, 35.41820216923952, 33.759296871721745, 36.17556393146515, 34.45229306817055, 36.14920563995838, 33.89862459152937, 37.65186294913292, 34.51096545904875, 37.78757341206074, 35.472409799695015, 35.691981203854084, 48.3900923281908, 49.765716306865215, 50.468217581510544, 46.91119771450758, 42.84156858921051, 36.741968244314194, 35.77661048620939, 37.10005525499582, 35.36489512771368, 38.98700326681137, 37.64844499528408, 36.357903853058815, 36.2352104857564, 42.43660066276789, 37.0072927325964, 35.5677530169487, 35.9690161421895, 38.793700747191906, 44.27275899797678, 38.566285744309425, 37.49627433717251, 38.55658043175936, 33.555708825588226, 38.438175804913044, 37.78866305947304, 36.95293329656124, 39.57269340753555, 38.537207059562206, 39.50682748109102, 36.296931095421314, 38.43045700341463, 39.03662506490946, 33.288439735770226, 38.457141257822514, 39.63425848633051, 34.96667928993702, 33.92667416483164, 38.841137662529945, 36.923933774232864, 37.79570944607258, 36.255937069654465, 38.02040498703718, 35.25926452130079, 33.50243158638477, 36.79124731570482, 37.761034443974495, 36.41999885439873, 49.45927765220404, 42.95017197728157, 43.65437850356102, 35.569856874644756, 34.53786764293909, 34.80852022767067, 33.39273948222399, 35.62125936150551, 38.30851800739765, 37.677776999771595, 36.17942053824663, 34.00070685893297, 34.301742911338806, 35.15278361737728, 35.60719080269337, 43.88647899031639, 39.897045120596886, 37.96092979609966, 34.86285265535116, 37.56320849061012, 34.08626560121775, 38.79082761704922, 44.55756675451994, 35.254862159490585, 36.979300901293755, 34.541258588433266, 34.99583434313536, 34.00609269738197, 35.08418332785368, 35.81689763814211, 37.78364695608616, 33.10783114284277, 37.60129678994417, 34.564959816634655, 35.23728158324957, 34.88949500024319, 35.43756250292063, 33.803464844822884, 37.88826987147331, 34.23675615340471, 34.16707552969456, 35.7371112331748, 35.20005289465189, 35.17123032361269, 36.25817969441414, 36.896517500281334, 33.9088374748826, 36.14241164177656, 43.046784587204456, 35.03971640020609, 42.49110538512468, 33.13351143151522, 36.40141058713198, 34.10730417817831, 37.28647902607918, 34.319658763706684, 36.99935879558325, 35.95582488924265, 35.595146007835865, 37.63184417039156, 35.97610257565975, 35.80732923001051, 36.412845365703106, 38.883560337126255, 42.127883061766624, 36.72497533261776, 38.01328502595425, 41.74785688519478, 34.15278717875481, 35.737534053623676, 35.64080595970154, 37.3539412394166, 38.22250943630934, 43.39610878378153, 36.61889210343361, 36.639331839978695, 39.5669424906373, 38.41965738683939, 41.90187994390726, 38.632615469396114, 35.86927056312561, 37.482915446162224, 37.56878059357405, 36.08329687267542, 36.17927432060242, 38.37365098297596, 39.067101664841175, 36.45051922649145, 37.70883847028017, 41.71001724898815, 39.77093379944563, 46.69445473700762, 42.391578666865826, 46.15581501275301, 36.98038961738348, 41.291882283985615, 36.58523689955473, 35.42476613074541, 43.22041664272547, 35.814751870930195, 36.613212898373604, 36.0894612967968, 34.65225826948881, 39.28772825747728, 42.237753979861736, 35.112286917865276, 36.508320830762386, 42.39704180508852, 34.08983442932367, 36.49757895618677, 38.32536470144987, 36.441946402192116, 35.39630398154259, 36.54182702302933, 37.84465231001377, 41.44019540399313, 36.100007593631744, 37.302713841199875, 37.802016362547874, 39.60696514695883, 38.47736120223999, 43.09336468577385, 36.93267051130533, 41.633373126387596, 36.506970413029194, 36.993011832237244, 37.417070008814335, 42.88806580007076, 37.80081681907177, 37.41749934852123, 35.787357948720455, 35.836693830788136, 44.291614554822445, 37.020440213382244, 36.19264252483845, 35.728043876588345, 37.17601019889116, 41.9701486825943, 34.59895495325327, 36.7850074544549, 34.23442132771015, 37.8146693110466, 38.34487870335579, 34.70742981880903, 37.83527389168739, 39.19337037950754, 34.991880878806114, 37.00978960841894, 39.25120551139116, 38.57077099382877, 43.024368584156036, 42.06267464905977, 45.27284111827612, 37.04253397881985, 42.471205815672874, 34.94822699576616, 33.08186586946249, 39.13091029971838, 35.57023871690035, 36.846840754151344, 36.28290630877018, 34.83618702739477, 35.74153408408165, 36.71683557331562, 37.55468688905239, 37.880685180425644, 35.74816416949034, 34.402516670525074, 38.02558220922947, 39.74706493318081, 36.71664651483297, 36.356003023684025, 36.07989847660065, 34.60499458014965, 34.666918218135834, 34.615871496498585, 37.26259618997574, 35.4810981079936, 38.36663160473108, 34.62045453488827, 34.51258409768343, 38.25636673718691, 36.077325232326984, 38.66676799952984, 44.236297719180584, 39.692698046565056, 38.72454911470413, 35.756636410951614, 35.313316620886326, 34.1457175090909, 35.546054132282734, 35.421084612607956, 34.15289707481861, </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -575,14 +683,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>{"classifier/VClassifier": {"config": {"INPUT_INFO": {"&lt;class 'list'&gt;": ["data"]}, "OUTPUT_INFO": "&lt;class 'list'&gt;", "input_shape": null, "output_shape": null}, "ppu_state": {"Classifier-resnet50/prepoc-resnet50": {"num_replicas": 3, "max_batch_size": 2, "resources": {"CPU1": 1}}, "Classifier-resnet50/model-resnet50": {"num_replicas": 1, "max_batch_size": 4, "resources": {"Tesla P40": 1}, "num_gpus": 1}}, "ppu_identifier": "Classifier-resnet50"}}</t>
+          <t>{"classifier/VClassifier": {"config": {"INPUT_INFO": {"&lt;class 'list'&gt;": ["data"]}, "OUTPUT_INFO": "&lt;class 'list'&gt;", "input_shape": null, "output_shape": null}, "ppu_state": {"Classifier-resnet34/prepoc-resnet34": {"num_replicas": 2, "max_batch_size": 5, "resources": {"CPU1": 1}}, "Classifier-resnet34/model-resnet34": {"num_replicas": 2, "max_batch_size": 2, "resources": {"Tesla P40": 1}, "num_gpus": 1}}, "ppu_identifier": "Classifier-resnet34"}}</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>91.30401587486267</v>
+        <v>71.74977540969849</v>
       </c>
       <c r="I2" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="J2" t="n">
         <v>75.8</v>
@@ -691,25 +799,25 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>91.30401587486267</v>
+        <v>71.74977540969849</v>
       </c>
       <c r="H2" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I2" t="n">
         <v>75.8</v>
       </c>
       <c r="J2" t="n">
-        <v>98.64415806724709</v>
+        <v>98.72854430192548</v>
       </c>
       <c r="K2" t="n">
-        <v>165.6768842078752</v>
+        <v>250.9694443212825</v>
       </c>
       <c r="L2" t="n">
-        <v>58.00230442546308</v>
+        <v>44.244787376374</v>
       </c>
       <c r="M2" t="n">
-        <v>65.11749558616428</v>
+        <v>52.89885649457573</v>
       </c>
     </row>
   </sheetData>
@@ -800,18 +908,594 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>91.30401587486267</v>
+        <v>71.74977540969849</v>
       </c>
       <c r="H2" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I2" t="n">
         <v>75.8</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[92.3042839858681, 93.35166896926239, 91.61052200943232, 88.40324700577185, 78.3912320039235, 90.59924504254013, 81.20116399368271, 71.53689296683297, 61.40011199750006, 68.58998001553118, 58.18657297641039, 49.59064000286162, 57.25336296018213, 47.21412499202415, 51.807935000397265, 44.01206102920696, 47.25650296313688, 55.674892966635525, 45.67858297377825, 51.22897296678275, 59.2611120082438, 49.64179900707677, 56.94496404612437, 47.01769701205194, 52.885267010424286, 58.432093006558716, 48.254609981086105, 56.38960900250822, 46.62068700417876, 51.92653398262337, 57.34474101336673, 48.09472797205672, 54.719470033887774, 44.33475900441408, 49.16375095490366, 56.96302198339254, 47.16692096553743, 53.399056021589786, 43.28543395968154, 45.918601972516626, 51.81608197744936, 42.69329801900312, 45.27363303350285, 52.69374401541427, 42.88080002879724, 46.59039399120957, 53.72097599320114, 43.97516301833093, 47.54901799606159, 69.2926969495602, 59.972854040097445, 70.12448698515072, 59.93877799483016, 51.00144003517926, 58.863290993031114, 49.05289801536128, 56.80243001552299, 47.05192300025374, 53.848849958740175, 44.561305025126785, 48.679692030418664, 55.05987303331494, 44.631526980083436, 50.85232597775757, 56.59912998089567, 47.14143800083548, 52.301486022770405, 60.37164700683206, 51.47746397415176, 55.07007701089606, 44.87431998131797, 52.75939998682588, 56.53358600102365, 46.7962310067378, 52.63545096386224, 62.20398499863222, 52.850842010229826, 60.11324003338814, 50.616135995369405, 65.98742603091523, 56.747880007606, 65.10381202679127, 54.7467460273765, 63.222228025551885, 54.260719974990934, 62.24066897993907, 53.02140803541988, 62.77082598535344, 53.063801024109125, 56.20169796748087, 45.448324002791196, 52.50632896786556, 59.99191600130871, 49.97419199207798, 57.184965000487864, 47.02633299166337, 52.934576000552624, 42.87775995908305, 47.4403869593516, 53.39985800674185, 44.07579603139311, 48.8813910051249, 57.35673400340602, 47.70252900198102, 53.15449903719127, 42.55338996881619, 48.6193360411562, 52.083023998420686, 43.936156027484685, 49.47183595504612, 58.23595600668341, 48.2598640373908, 53.84112102910876, 44.1477739950642, 49.213752965442836, 54.90824399748817, 45.27998901903629, 52.45624401140958, 59.025685011874884, 52.94800299452618, 56.598935974761844, 47.947831044439226, 53.91393601894379, 44.341889035422355, 48.80760802188888, 56.32766603957862, 46.430650050751865, 49.789725977461785, 55.353947973344475, 63.53642599424347, 53.97422797977924, 58.878201991319656, 50.31875096028671, 58.1406140117906, 48.43138996511698, 53.51416498888284, 43.95780200138688, 47.53301903838292, 53.47832798724994, 43.74133300734684, 48.36129199247807, 55.53598399274051, 46.36239499086514, 52.32907703612, 57.4411730049178, 47.6966819842346, 53.049260983243585, 43.4813269530423, 47.576508950442076, 55.56046596029773, 45.07594305323437, 51.771115977317095, 58.68605099385604, 49.057219992391765, 58.32007800927386, 72.78623199090362, 63.08555603027344, 75.29542100382969, 65.78798999544233, 55.98498199833557, 62.892650021240115, 53.58306196285412, 59.5158800133504, 49.57076703431085, 58.71001398190856, 49.00339001324028, 56.21727800462395, 46.973933989647776, 52.71237000124529, 62.488631054293364, 52.74298903532326, 57.43543297285214, 47.57936799433082, 53.040196013171226, 43.567831977270544, 48.28946205088869, 52.86791699472815, 44.22142496332526, 49.02574303559959, 51.91937094787136, 43.161141977179796, 47.40441497415304, 53.35492501035333, 43.72547002276406, 47.51918202964589, 53.598837985191494, 43.9657749957405, 49.39996497705579, 56.422891037072986, 46.608456992544234, 51.99546198127791, 41.247525019571185, 52.67488397657871, 62.20456800656393, 52.47471801703796, 58.533337025437504, 48.181620019022375, 54.32395898969844, 63.2755879778415, 53.63363097421825, 59.5016639563255, 49.16145099559799, 55.941211991012096, 46.199126983992755, 52.58647201117128, 57.20719299279153, 47.12279397062957, 52.68999299732968, 61.73008598852903, 52.44813300669193, 57.613431999925524, 47.92906396323815, 52.082473994232714, 43.25083101866767, 47.98372701043263, 52.91550501715392, 43.35341998375952, 47.579874051734805, 52.85279802046716, 43.67253399686888, 48.23614901397377, 53.81828505778685, 43.45400497550145, 47.97840700484812, 53.747832018416375, 44.6335319429636, 49.12528395652771, 56.43083294853568, 47.44711297098547, 51.884601009078324, 42.09226596867666, 47.247303009498864, 53.81918099010363, 44.00008701486513, 47.36093699466437, 53.433406981639564, 43.539446021895856, 46.917962026782334, 53.416473034303635, 44.05032395152375, 48.63218800164759, 56.385739997494966, 46.849049045704305, 52.628943987656385, 42.43847797624767, 46.21359001612291, 52.23178898449987, 42.4278219579719, 45.542264997493476, 51.56700900988653, 57.604899047873914, 48.72675699880347, 55.106560001149774, 45.84495699964464, 52.83931200392544, 58.567505970131606, 49.34695997508243, 55.974007002078, 46.14978900644928, 51.65811098413542, 62.079562980216, 52.85278201336041, 56.44688301254064, 46.99472099309787, 53.30728000262752, 57.921188010368496, 48.762220016215, 56.250382971484214, 46.44809302408248, 51.82889802381396, 42.35046997200698, 48.514747992157936, 56.97437503840774, 47.7772899903357, 55.64959300681949, 45.03870400367305, 50.636388012208045, 58.15748200984672, 48.183387028984725, 53.4118739888072, 44.34636601945385, 47.68808896187693, 54.157121980097145, 45.34503899049014, 52.5703530292958, 57.34786996617913, 48.31838503014296, 56.675655010621995, 46.75687098642811, 52.68414400052279, 42.82798897475004, 45.63801200129092, 52.38425201969221, 41.97044397005811, 46.797501971013844, 53.304744011256844, 44.1338189993985, 48.706767964176834, 55.10052101453766, 52.332211984321475, 52.282331977039576, 54.641022987198085, 45.53549800766632, 49.50702399946749, 51.501162990462035, 45.610854984261096, 49.449393001850694, 55.05890998756513, 45.18852400360629, 50.253748951945454, 56.120402994565666, 45.87155004264787, 51.265304966364056, 57.20823904266581, 47.00442001922056, 51.974712987430394, 42.80145699158311, 44.42925099283457, 52.68884199904278, 42.72938298527151, 46.391978044994175, 52.349414967466146, 42.94186003971845, 46.892773010767996, 53.07126702973619, 43.146025971509516, 47.204701986629516, 52.00056597823277, 43.23813098017126, 48.822822980582714, 52.683836955111474, 43.27569901943207, 48.87857200810686, 53.59763198066503, 44.418703007977456, 47.68032894935459, 52.335679007228464, 42.32890997081995, 52.91080998722464, 63.180928002111614, 53.494919964578, 59.609312971588224, 52.45522496988997, 57.22364998655394, 47.25169396260753, 52.928494988009334, 43.60760102281347, 46.99490696657449, 52.44589998619631, 42.475523019675165, 45.50400498555973, 52.51883500022814, 42.622296954505146, 46.398031001444906, 52.37453797599301, 42.63203497976065, 46.03774001589045, 52.91773995850235, 42.94254595879465, 45.635659946128726, 52.01632500393316, 42.716013034805655, 43.11949299881235, 49.05817599501461, 55.12787599582225, 44.90307200467214, 52.37490602303296, 57.530838006641716, 47.67879098653793, 53.49257303168997, 43.58576197410002, 45.64977594418451, 52.18716600211337, 56.311076041311026, 46.79880401818082, 52.64686496229842, 43.11116301687434, 44.94711197912693, 52.65640397556126, 56.819046032615006, 47.28559899376705, 52.8152710176073, 62.19732097815722, 52.910232974682, 56.11608497565612, 48.078979016281664, 54.194653988815844, 44.43399398587644, 48.4146429807879, 56.677618995308876, 47.136866953223944, 53.572801989503205, 43.021377990953624, 48.06670802645385, 56.627311976626515, 46.77950398763642, 52.48436098918319, 43.58371201669797, 47.55930998362601, 55.16028095735237, 45.34109903033823, 49.681988020893186, 56.04511097772047, 47.09258204093203, 52.49609804013744, 42.325203015934676, 45.93837499851361, 53.871915966738015, 44.311589968856424, 49.18020695913583, 54.19578100554645, 44.40629098098725, 49.19904196867719, 55.1776880165562, 45.24318396579474, 52.66537802526727, 57.22149700159207, 47.53842402715236, 53.66726097417995, 43.919892981648445, 48.777617048472166, 54.706706025172025, 44.89690699847415, 50.14457396464422, 58.148037001956254, 48.416982986964285, 55.98541704239324, 46.05121701024473, 52.97125602373853, 43.29157096799463, 47.8154779993929, 56.211623013950884, 46.237338974606246, 52.39117401652038, 42.681842984165996, 46.8374959891662, 54.45283296285197, 44.71102199750021, 49.341711041051894, 54.4745369697921, 44.67811301583424, 48.992243013344705, 56.66741298045963, 46.90996598219499, 54.33356197318062, 44.403770996723324, 49.1298510460183, 57.52685200423002, 47.70555498544127, 54.811128007713705, 45.41193100158125, 52.21699899993837, 56.80729099549353, 47.99390700645745, 54.46881300304085, 44.679813960101455, 49.286914989352226, 55.04166998434812, 45.215738005936146, 52.476359996944666, 61.64374103536829, 52.441495994571596, 52.176891011185944, 43.10115100815892, 47.95390396611765, 53.74498898163438, 42.24571801023558, 49.70489797415212, 56.363956013228744, 46.61333101103082, 52.529830019921064, 42.64025099109858, 45.90441798791289, 53.07942599756643, 43.224185006693006, 46.23517603613436, 52.46438801987097, 43.33499097265303, 46.09418602194637, 52.39545804215595, 42.6375949755311, 46.4292989927344, 52.16376902535558, 56.35425099171698, 47.79126401990652, 53.04699100088328, 56.47232901537791, 47.35109698958695, 52.46933799935505, 62.577482021879405, 51.70435702893883, 57.64596303924918, 48.25418203836307, 53.5291830310598, 42.92603599606082, 47.593866009265184, 52.97773901838809, 43.74955396633595, 48.56965900398791, 53.13662299886346, 43.491913995239884, 47.725307988002896, 52.9362759552896, 43.8501019962132, 50.365759001579136, 56.92829203326255, 47.10655799135566, 52.64547799015418, 42.9261940298602, 44.72899198299274, 50.3802290186286, 57.647778012324125, 48.65138197783381, 54.5836899545975, 45.193535974249244, 48.33974497159943, 57.45955801103264, 47.6978020160459, 52.695543970912695, 43.04854100337252, 46.43381998175755, 52.80241201398894, 42.90250298799947, 47.26224596379325, 53.65118698682636, 43.90544904163107, 51.87681003008038, 56.444810004904866, 46.45416705170646, 51.688274019397795, 42.78246499598026, 46.66133300634101, 56.1159829958342, 46.19436099892482, 52.319251000881195, 42.41904499940574, 46.6488900128752, 50.97807297715917, 42.66408900730312, 47.13056900072843, 53.782778966706246, 44.31370896054432, 48.306797980330884, 56.49239895865321, 46.70832498231903, 53.03903802996501, 43.19440800463781, 46.321059053298086, 51.717261027079076, 57.84708197461441, 47.26513900095597, 54.16821897961199, 44.387536006979644, 49.15102198719978, 55.7035889942199, 45.91484903357923, 52.39978799363598, 42.54864202812314, 44.89092901349068, 51.62514897529036, 42.551108985207975, 45.67043198039755, 51.508684002328664, 42.523924028500915, 46.533854969311506, 52.703873021528125, 43.10757794883102, 47.19765798654407, 54.054923995863646, 44.93483598344028, 49.6684749959968, 56.46107898792252, 47.14699101168662, 54.20637194765732, 43.43475797213614, 48.54677099501714, 53.21882799034938, 43.769392010290176, 47.597552998922765, 53.50539099890739, 44.37781503656879, 48.373110010288656, 53.705648984760046, 44.11221400368959, 48.377342987805605, 54.791205970104784, 45.848395966459066, 52.857325004879385, 43.154622020665556, 46.96219804463908, 52.579804963897914, 42.78322501340881, 47.192764992360026, 52.61624098056927, 42.78929199790582, 47.284787986427546, 53.47490403801203, 42.875427985563874, 46.89330101246014, 52.29340703226626, 42.380753031466156, 47.2351839998737, 52.42382502183318, 43.198362982366234, 47.21556603908539, 53.26448701089248, 43.56124298647046, 46.76172899780795, 51.400961994659156, 42.5305999815464, 45.923216035589576, 52.353537001181394, 42.37514903070405, 46.46204796154052, 52.845091035123914, 42.90673101786524, 45.4945900128223, 52.41212801774964, 58.397773012984544, 48.957256018184125, 54.840028984472156, 45.378571026958525, 52.405316033400595, 42.58950398070738, 45.493300014641136, 50.514945993199944, 41.1354840034619, 44.145512976683676, 49.57128502428532, 57.278938009403646, 46.094955992884934, 51.58485297579318, 42.45282802730799, 46.96187499212101, 52.18279198743403, 42.573979997541755, 47.30383103014901, 52.81860800459981, 42.97225101618096, 47.291929950006306, 54.21525699784979, 43.63098699832335, 49.11466798512265, 57.16565699549392, 47.4172790418379, 52.89413098944351, 42.96444699866697, 47.26452601607889, 56.09109398210421, 46.1774249561131, 53.456040972378105, 43.53686299873516, 44.38354098238051, 51.52899300446734, 57.749287982005626, 46.383840031921864, 54.12207200424746, 44.11175602581352, 48.87337499530986, 55.85499701555818, 46.036494022700936, 52.306202007457614, 42.7789959940128, 47.04087303252891, 53.38884796947241, 44.12610997678712, 47.743223956786096, 54.65335998451337, 44.628404022660106, 48.67749201366678, 55.92056200839579, 47.2411600057967, 52.606721001211554, 42.433467984665185, 47.21076402347535, 54.34533196967095, 44.18900900054723, 48.9945329609327, 57.547471951693296, 47.86235501524061, 54.747701971791685, 43.80008002044633, 49.62642601458356, 58.82209003902972, 49.648569023702294, 56.678275985177606, 46.26715602353215, 53.833644022233784, 44.07716600690037, 49.07593398820609, 56.0930929495953, 46.1087939911522, 52.26847401354462, 56.10776599496603, 47.13436798192561, 55.655370000749826, 46.3471130351536, 53.503512986935675, 44.057766965124756, 48.59318595845252, 57.059673010371625, 47.19914402812719, 56.50850897654891, 46.82805301854387, 54.38257899368182, 44.433912029489875, 48.40825201245025, 55.85223302477971, 46.68069601757452, 53.199552989099175, 44.659175036940724, 47.49596200417727, 55.28436996974051, 45.35905900411308, 53.28415596159175, 57.643248001113534, 47.208660980686545, 55.124795995652676, 45.757172047160566, 51.39843397773802, 42.31300996616483, 45.71686597773805, 52.47708299430087, 42.66128002200276, 46.61443695658818, 52.71766899386421, 42.58990997914225, 47.46829898795113, 53.606006025802344, 44.25422300118953, 49.06333895632997, 55.53969496395439, 45.574424031656235, 51.67297803563997, 42.7723930333741, 44.960332044865936, 50.141782965511084, 55.374135030433536, 46.14444397157058, 51.68913403758779, 43.1809849687852, 47.118449001573026, 53.268907009623945, 43.76557801151648, 47.16707702027634, 52.279750001616776, 43.170624994672835, 47.02088498743251, 53.11492003966123, 62.37194803543389, 51.928719971328974, 57.818740024231374, 47.91118297725916, 53.464393015019596, 43.8545539509505, 46.79970699362457, 52.93293599970639, 43.19404100533575, 46.955491008702666, 51.64084496209398, 60.76741102151573, 51.03379499632865, 57.64687299961224, 47.77135397307575, 53.21586097124964, 43.23036503046751, 46.28451599273831, 52.62605397729203, 42.292160040233284, 45.86211603600532, 51.80351104354486, 42.483686993364245, 45.88201601291075, 51.869768009055406, 42.9914589622058, 46.06732400134206, 50.61542900511995, 42.64613601844758, 45.91028799768537, 52.02098796144128, 42.66811703564599, 45.63948599388823, 52.49911599094048, 42.61010797927156, 45.024419960100204, 50.27054401580244, 55.82191701978445, 46.99596099089831, 52.03205603174865, 42.844494979362935, 45.12060194974765, 52.4700140231289, 42.62023197952658, 45.12067302130163, 51.987309008836746, 58.77197696827352, 49.00984599953517, 56.62531696725637, 45.889845001511276, 52.98511200817302, 42.800360010005534, 47.686819976661354, 54.44642098154873, 44.06831203959882, 49.099138006567955, 54.727584996726364, 45.12441600672901, 52.42781498236582, 58.098274981603026, 48.443039995618165, 55.21144298836589, 44.396283046808094, 52.25928401341662, 57.55530402529985, 48.262458003591746, 54.60739502450451, 44.59578695241362, 48.4555930015631, 56.07026600046083, 46.87664599623531, 52.45367897441611, 42.553342995233834, 46.334148035384715, 52.13044595438987, 42.9073820123449, 47.62578697409481, 55.64690299797803, 44.62540696840733, 52.442395011894405, 57.352670992258936, 47.68246097955853, 53.24239103356376, 44.0626289928332, 49.280075007118285, 54.23729697940871, 45.12776399496943, 49.05017599230632, 56.663530005607754, 46.91570298746228, 52.779032033868134, 42.998362972866744, 47.22649202449247, 54.9517449690029, 44.5118680363521, 52.40756704006344, 56.55694397864863, 47.371276014018804, 54.34672097908333, 44.65375101426616, 48.821820004377514, 55.84522697608918, 45.960395014844835, 51.24739900929853, 57.52649100031704, 47.71607898874208, 53.80512500414625, 44.61519100004807, 50.68239400861785, 56.210296985227615, 46.58139497041702, 52.874447021167725, 42.84454201115295, 46.727441949769855, 52.63962101889774, 43.08679100358859, 48.78196498611942, 55.35082204733044, 46.13002797123045, 52.22385301021859, 57.60438699508086, 47.698677983134985, 53.00475098192692, 44.2318829591386, 49.04746502870694, 53.31022199243307, 43.80945098819211, 48.91487100394443, 53.04383800830692, 43.866644031368196, 47.76190099073574, 52.473818010184914, 43.295442999806255, 47.34843800542876, 52.55697900429368, 42.74578596232459, 49.04454597271979, 53.49211301654577, 44.78097194805741, 49.242014007177204, 54.69118698965758, 45.61539797578007, 52.32964496826753, 57.05954000586644, 47.164275019895285, 52.55183100234717, 42.88009298034012, 47.21723799593747, 53.198861016426235, 43.50251698633656, 47.411992971319705, 51.867964037228376, 42.00157802551985, 47.213312005624175, 53.233726997859776, 43.214857985731214, 47.37468098755926, 52.54596198210493, 43.177289015147835, 47.24118299782276, 52.56909300806001, 42.77400398859754, 47.024441009853035, 53.23109496384859, 43.693040031939745, 47.15456202393398, 52.96073399949819, 43.24104799889028, 45.76127097243443, 53.0998469912447, 43.24323101900518, 46.91474500577897, 52.27665702113882, 42.743890022393316, 46.86155600938946, 51.945446990430355, 42.814382002688944, 47.535244026221335, 53.04211500333622, 43.358791968785226, 47.941701021045446, 54.92413102183491, 45.247275033034384, 52.15753195807338, 56.58919096458703, 45.57287797797471, 52.793767012190074, 42.282590991817415, 46.90406797453761, 54.34585199691355, 44.41863700048998, 49.8390169814229, 60.76179299270734, 52.62239504372701, 59.187020000535995, 50.040159025229514, 56.736471015028656, 63.668430026154965, 53.482596995308995, 62.38929199753329, 51.729788014199585, 58.009742002468556, 47.542682965286076, 54.991670011077076, 45.14371801633388, 52.668431017082185, 42.9686950519681, 43.279209989123046, 49.63211598806083, 52.09036997985095, 44.82128599192947, 49.164949043188244, 56.615289009641856, 46.58381000626832, 52.29273403529078, 42.71440498996526, 45.05357699235901, 52.29182698531076, 56.379897985607386, 48.16504701739177, 54.63620997034013, 44.54860900295898, 48.76550001790747, 39.06005498720333, 44.991770992055535, 52.39690002053976, 42.408092005643994, 44.94174203136936, 51.56613403232768, 42.51430300064385, 43.2459200383164, 48.718237958382815, 52.67554504098371, 43.24636101955548, 46.721514023374766, 53.02074801875278, 44.0916339866817, 48.74531098175794, 56.30203697364777, 46.380928019061685, 52.32297000475228, 41.67659400263801, 46.14492895780131, 52.734842989593744, 42.92145697399974, 46.32538201985881, 52.598572976421565, 42.801506991963834, 46.80430598091334, 54.34124602470547, 43.24125801213086, 48.548606981057674, 54.665503033902496, 45.53234501508996, 52.49390401877463, 42.54766902886331, 44.370171963237226, 52.238935022614896, 42.2570810187608, 43.2716510258615, 47.57985600735992, 53.88752301223576, 44.25282997544855, 48.78399602603167, 55.26187899522483, 44.312355981674045, 52.44087299797684, 42.47572994790971, 45.1528379926458, 52.33835196122527, 42.49299404909834, 45.48862297087908, 52.88348800968379, 42.446210980415344, 46.64561996469274, 52.938968990929425, 43.248527974355966, 47.22346999915317, 53.312441043090075, 43.62378403311595, 47.928387008141726, 54.423195018898696, 43.77562599256635, 48.06350701255724, 53.3093570265919, 44.13880896754563, 49.75869000190869, 55.65663700690493, 45.82294699503109, 52.060677960980684, 42.360874998848885, 46.437370008789, 51.53657600749284, 42.189198022242635, 46.176219009794295, 51.49122601142153, 42.82280901679769, 46.28202703315765, 52.33772599603981, 42.3202840029262, 45.32852198462933, 51.08871002448723, 42.482424003537744, 42.92009002529085, 48.17649401957169, 52.779764984734356, 43.699366971850395, 48.0467050219886, 52.54312901524827, 60.042052005883306, 50.13977299677208, 55.741766991559416, 45.97881104564294, 52.194088988471776, 41.82561603374779, 44.864557043183595, 50.91567902127281, 42.24390600575134, 45.00132397515699, 51.99841700959951, 42.094318952877074, 45.646447979379445, 52.019077993463725, 42.32311301166192, 45.853716030251235, 52.4212809978053, 42.51106298761442, 45.68562301574275, 51.757067965809256, 42.34574898146093, 44.56876200856641, 48.615872976370156, 52.74408601690084, 62.475017039105296, 70.45939902309328, 62.10181099595502, 53.113922011107206, 56.26962200039998, 63.68231697706506, 53.71839401777834, 58.80221200641245, 49.00737601565197, 55.73724501300603, 45.935930975247175, 49.077241972554475, 56.51697498979047, 47.31964005623013, 52.368317963555455, 41.950806975364685, 46.239199000410736, 52.52146703423932, 41.81035602232441, 45.69753899704665, 52.340857044328004, 42.49932599486783, 45.420780952554196, 52.33587202383205, 42.31398901902139, 45.36507203010842, 48.861071991268545, 39.56554603064433, 43.903914047405124, 49.36568101402372, 55.359609017614275, 45.344844984356314, 49.58934703608975, 40.28165194904432, 43.45569701399654, 49.175330030266196, 55.188445025123656, 46.482369012665, 52.49684303998947, 57.71752499276772, 48.4027789789252, 53.248846961651, 59.007273986935616, 49.84820896061137, 54.41503401380032, 44.02084700996056, 48.97492699092254, 54.81929401867092, 45.618203992489725, 50.30614498537034, 56.4377800328657, 47.43579699425027, 53.21877798996866, 44.76587497629225, 50.05954799707979, 55.98608998116106, 46.244680997915566, 53.59818396391347, 62.809914990793914, 52.635714993812144, 58.97587304934859, 49.29566098144278, 54.32565597584471, 44.24550797557458, 49.52924099052325, 54.30149903986603, 44.90385000826791, 50.42271100683138, 56.05775600997731, 46.21637595118955, 52.37148003652692, 56.90067895920947, 46.63837299449369, 49.539777042809874, 57.04958300339058, 47.20497695961967, 53.01796202547848, 43.16649597603828, 46.45692399935797, 53.98148304084316, 44.08210696419701, 47.488854033872485, 53.94565802998841, 43.59930503414944, 47.0820150221698, 53.98765200516209, 44.15946500375867, 49.36584999086335, 54.267192957922816, 44.584852003026754, 48.33013197639957, 54.32649696012959, 44.54987298231572, 49.682009033858776, 55.69631600519642, 45.930081978440285, 51.96560698095709, 42.5981690059416, 46.18019802728668, 52.47496999800205, 42.738113028462976, 46.526541002094746, 52.442778018303216, 58.00147802801803, 50.12549803359434, 53.46017802366987, 43.63872401881963, 48.03803999675438, 52.25669400533661, 42.98914800165221, 47.399075992871076, 54.16216095909476, 44.34410796966404, 48.98996598785743, 57.38729302538559, 47.63669898966327, 53.035219956655055, 43.04386401781812, 47.08265303634107, 51.52374098543078, 42.57132497150451, 46.67800001334399, 52.879105031024665, 42.52104100305587, 46.580394031479955, 52.58366197813302, 42.619272018782794, 44.8162829852663, 50.79893599031493, 57.306900969706476, 47.48947999905795, 52.158289996441454, 42.56843600887805, 45.70786497788504, 52.41804197430611, 42.593150050379336, 46.362480032257736, 51.382953010033816, 42.23049501888454, 46.04466701857746, 52.13440296938643, 42.1682620071806, 45.57924496475607, 51.68814095668495, 42.32411296106875, 45.6707279663533, 52.2768379887566, 42.300550965592265, 45.14134599594399, 52.413308003451675, 42.610955017153174, 44.03622401878238, 49.075611983425915, 56.794465985149145, 46.53266497189179, 51.42870597774163, 42.45092102792114, 46.008003992028534, 51.03398801293224, 58.33505996270105, 48.64926100708544, 52.64037003507838, 43.26123802457005, 46.266763005405664, 53.309253009501845, 43.72887301724404, 48.028221004642546, 53.546506038401276, 43.723752023652196, 49.70618797233328, 56.34205398382619, 46.53047799365595, 52.11357999360189, 43.32842800067738, 46.70875205192715, 52.62898199725896, 42.790847015567124, 45.5847880220972, 52.47060599504039, 56.62002501776442, 47.4361430387944, 53.9248589775525, 44.40171702299267, 48.352740006521344, 57.23028298234567, 47.34477901365608, 53.823510999791324, 43.946678983047605, 47.43311298079789, 53.34902001777664, 44.82034099055454, 49.671108019538224, 56.8795150029473, 46.99890699703246, 54.13770896848291, 45.17641704296693, 48.43724297825247, 56.8533840123564, 47.03993705334142, 52.4923000484705, 42.09370800526813, 46.70957999769598, 52.450191986281425, 43.70076098712161, 47.99026303226128, 55.27923000045121, 45.49004201544449, 50.02533900551498, 56.11699598375708, 47.106718993745744, 53.41478402260691, 43.60628401627764, 48.18420100491494, 55.52280502161011, 46.39705101726577, 52.2227410110645, 42.4096190254204, 46.60658701322973, 52.775891963392496, 43.04095800034702, 46.809474006295204, 53.9014259702526, 44.33729499578476, 50.0265330192633, 56.60942802205682, 46.71063896967098, 53.743685013614595, 43.901675962843, 48.19678299827501, 55.88220799108967, 46.17612098809332, 52.66092100646347, 42.33043297426775, 45.20059801870957, 52.19892895547673, 42.66814701259136, 46.41401598928496, 52.01166699407622, 44.060683983843774, 47.000133024994284, 52.780222962610424, 43.29934099223465, 45.39909400045872, 53.056049975566566, 43.92212600214407, 48.87819499708712, 53.2296160236001, 43.17072301637381, 48.52859099628404, 53.99022396886721, 44.21559703769162, 48.18288004025817, 53.76643198542297, 44.68083300162107, 51.74966901540756, 56.61503301234916, 46.98179999832064, 55.28247001348063, 45.40475702378899, 52.96270898543298, 53.710760024841875, 44.734555995091796, 49.524777045007795, 54.98633801471442, 44.79527805233374, 51.76740902243182, 57.03443998936564, 47.234120953362435, 54.19803800759837, 44.55998196499422, 49.145297962240875, 54.107024043332785, 44.918967003468424, 48.99997700704262, 55.27251900639385, 43.822836014442146, 52.27247398579493, 42.40501200547442, 45.49185204086825, 52.851043990813196, 42.933032964356244, 44.20088202459738, 48.16170100821182, 53.933083021547645, 44.16905203834176, 48.53555402951315, 54.516601958312094, 44.63992896489799, 48.72486100066453, 56.05593300424516, 46.318162989337, 52.071411977522075, 42.18332300661132, 45.55922403233126, 51.01545201614499, 58.43986303079873, 49.24926802050322, 54.005350975785404, 44.08878198591992, 48.78043697681278, 54.4006850104779, 44.49758102418855, 49.43103302503005, 54.29847602499649, 44.5964329992421, 51.5850959927775, 55.788061989005655, 45.94349500257522, 53.62911301199347, 56.57908698776737, 46.82009998941794, 52.180183003656566, 42.47402003966272, 44.78738101897761, 51.61994299851358, 41.69979802099988, 44.87030697055161, 50.21030403440818, 56.70095497043803, 46.789246960543096, 52.895455970428884, 42.90082002989948, 44.639684027060866, 48.73655299888924, 56.11949000740424, 46.76681698765606, 51.50557402521372, 42.41263901349157, 44.21559302136302, 47.916984010953456, 50.581321003846824, 42.728856031317264, 47.00260696699843, 52.95132799074054, 42.4603009596467, 46.27573996549472, 52.272032015025616, 42.392629955429584, 45.00639199977741, 52.06962797092274, 42.1930740121752, 43.48290798952803, 49.09329896327108, 55.90223299805075, 46.14168300759047, 50.25077803293243, 40.62146000796929, 43.04092098027468, 45.16738199163228, 54.04596001608297, 43.915096030104905, 49.42645295523107, 56.556515977717936, 46.61836696323007, 52.52224096329883, 42.85792098380625, 47.12503700284287, 54.45832299301401, 44.12234597839415, 49.53958099940792, 56.481795967556536, 46.68342799413949, 53.93565498525277, 44.0367300179787, 46.61250300705433, 52.52209003083408, 42.688092042226344, 45.317062991671264, 51.932276983279735, 42.77422197628766, 46.950425021350384, 53.32916998304427, 43.78812602953985, 47.47730598319322, 54.16053900262341, 44.41154602682218, 48.19877998670563, 55.19060796359554, 45.580014993902296, 49.48122502537444, 55.639492988120764, 46.67846002848819, 53.19350096397102, 43.45693998038769, 46.234602050390095, 52.677929983474314, 42.638135026209056, 45.19448400242254, 52.50581604195759, 42.69090102752671, 45.49181601032615, 51.92286102101207, 43.56063000159338, 46.56141699524596, 52.72066697943956, 43.002827966120094, 46.8072280054912, 52.75341996457428, 42.952353018336, 44.85658201156184, 50.026069045998156, 56.85349297709763, 46.893931983504444, 55.691205023322254, 46.24474002048373, 51.305561035405844, 42.596727958880365, 46.126394998282194, 53.22866200003773, 43.262396997306496, 47.60777699993923, 55.86710898205638, 45.97765998914838, 51.85096198692918, 42.66069398727268, 45.86570302490145, 52.39979602629319, 42.33756597386673, 45.37312802858651, 52.268858009483665, 42.655967990867794, 45.49259098712355, 52.386442956048995, 56.03364302078262, 46.135124983265996, 50.86948600364849, 60.011197987478226, 50.41041801450774, 54.8619200126268, 44.831678038463, 50.62398599693552, 56.67662597261369, 46.39959702035412, 53.674584021791816, 43.913763016462326, 45.70502298884094, 52.264500001911074, 43.30059501808137, 47.03323298599571, 52.68122802954167, 42.667234025429934, 47.29480901733041, 52.388174983207136, 42.84622997511178, 47.17031097970903, 50.558459013700485, 42.58489503990859, 46.86940595274791, 51.383911981247365, 42.55861300043762, 47.23644396290183, 52.967889001592994, 42.9775639786385, 47.95299400575459, 58.99182701250538, 49.32779399678111, 54.30784996133298, 43.915638991165906, 52.55524400854483, 48.27321198536083, 58.62543999683112, 52.77750897221267, 61.49420398287475, 52.46069299755618, 58.715457969810814, 49.58852502750233, 55.54269801359624, 45.97042698878795, 52.76293499628082, 42.83985897200182, 46.115435019601136, 52.84626595675945, 42.96710202470422, 46.04052199283615, 52.78707901015878, 42.8430309984833, 46.75033700186759, 53.048410976771265, 44.40844798227772, 50.166522967629135, 55.70777301909402, 46.71136196702719, 52.681695960927755, 43.065692007075995, 44.799244962632656, 52.5694009847939, 58.5390769992955, 48.567209974862635, 52.52893303986639, 43.09430002467707, 48.41042298357934, 54.742335982155055, 44.898442982230335, 49.918197037186474, 57.41496797418222, 47.933014982845634, 53.02924202987924, 44.126375985797495, 48.58760099159554, 56.1904109781608, 46.3636209606193, 51.33053701138124, 42.18430502805859, 46.31051199976355, 52.312766027171165, 42.47374401893467, 45.795570011250675, 50.6307749892585, 42.707922984845936, 45.07532197749242, 50.36224698415026, 58.367166959214956, 47.81021300004795, 56.68820004211739, 46.75311199389398, 51.77440302213654, 42.57043299730867, 45.62853300012648, 52.367322030477226, 58.742071967571974, 49.42743299761787, 53.699826006777585, 44.85949804075062, 48.63940901122987, 54.1077220113948, 44.46806799387559, 49.37139298999682, 55.4673449951224, 45.62197002815083, 49.86466799164191, 57.61306901695207, 47.766358009539545, 54.11141301738098, 44.46254501817748, 48.740687023382634, 56.27048300812021, 46.37871799059212, 52.78922204161063, 43.024084996432066, 46.78279400104657, 52.326432953123, 41.64387797936797, 47.08053998183459, 52.295703964773566, 42.786876030731946, 46.676263969857246, 52.744855056516826, 43.12121600378305, 47.69920400576666, 55.34203496063128, 45.47764197923243, 49.601417966187, 56.46512197563425, 46.68416199274361, 53.175501991063356, 43.72914903797209, 47.69880301319063, 53.9501229650341, 44.1115060239099, 47.817900020163506, 52.968965959735215, 42.64115000842139, 47.73482901509851, 54.553456022404134, 44.85983500489965, 49.43749797530472, 56.038597016595304, 46.18304001633078, 54.03501295950264, 44.30711199529469, 48.4044459881261, 53.990119020454586, 43.75098698073998, 48.85370604461059, 54.195388045627624, 44.39092200482264, 48.56289702001959, 54.697898973245174, 45.17768102232367, 52.38410900346935, 55.230188998393714, 45.5330690019764, 48.93069399986416, 54.99617598252371, 46.09913000604138, 53.29026095569134, 43.50033600348979, 45.47775100218132, 52.52369504887611, 42.707200977019966, 44.35607703635469, 49.04846899444237, 53.68474300485104, 44.6941260015592, 50.61922699678689, 54.823181009851396, 45.33963795984164, 52.68402799265459, 57.58099997183308, 47.104981960728765, 53.75280597945675, 43.397331959567964, 47.280828992370516, 51.975819980725646, 42.87875699810684, 45.722631039097905, 52.60765599086881, 43.04629797115922, 46.75707302521914, 52.63524403562769, 42.812585015781224, 46.778880001511425, 52.637866989243776, 42.83312801271677, 44.728389009833336, 48.260774987284094, 56.563777034170926, 46.793218003585935, 51.938120974227786, 42.11112397024408, 45.81159696681425, 53.44315699767321, 43.516019999515265, 47.2201029770076</t>
-        </is>
+          <t>[71.49561867117882, 51.68141983449459, 54.98585291206837, 77.02314760535955, 78.33578251302242, 88.53293675929308, 79.57708649337292, 74.968914501369, 66.54954608529806, 65.66909234970808, 55.497607216238976, 47.576699405908585, 50.72555597871542, 43.25151536613703, 37.04150207340717, 36.589790135622025, 35.291582345962524, 36.64617333561182, 35.42403969913721, 36.44913528114557, 35.23509856313467, 36.33748274296522, 35.08493211120367, 36.478519439697266, 35.10662354528904, 36.27839218825102, 35.503171384334564, 36.31517384201288, 35.47608759254217, 36.291783675551414, 35.83159018307924, 36.24401148408651, 35.63260566443205, 35.84972582757473, 34.61418393999338, 35.425146110355854, 36.485178396105766, 35.58931965380907, 36.84348240494728, 33.94585754722357, 40.114798583090305, 34.93273723870516, 37.375844083726406, 35.57120729237795, 38.99080399423838, 37.634337320923805, 38.071829825639725, 38.084592670202255, 41.44783038645983, 38.65957912057638, 37.148285657167435, 37.30161860585213, 39.16363790631294, 37.49328479170799, 42.101964354515076, 38.98073732852936, 41.079808957874775, 38.79270423203707, 38.66849932819605, 38.29483035951853, 36.90842725336552, 44.53947115689516, 37.065944634377956, 48.28481934964657, 35.3426281362772, 44.06313318759203, 34.729281440377235, 37.11697831749916, 36.54366731643677, 37.109251134097576, 38.078274577856064, 37.05791477113962, 37.73552365601063, 37.53458149731159, 39.51473534107208, 37.86760289222002, 37.357558496296406, 38.65246847271919, 42.5570672377944, 39.33619521558285, 37.28192858397961, 37.92671859264374, 44.83048431575298, 37.43425756692886, 41.82071704417467, 36.46683506667614, 35.05858592689037, 39.42856192588806, 39.03398662805557, 37.27692924439907, 43.06055046617985, 37.58459724485874, 41.25696327537298, 36.82637307792902, 35.6726348400116, 37.58584149181843, 42.13381186127663, 52.675243467092514, 42.12247580289841, 37.93713636696339, 42.7912725135684, 36.2639706581831, 50.59358756989241, 36.71893756836653, 42.986998334527016, 36.508974619209766, 40.21841753274202, 45.03596015274525, 36.466075107455254, 36.01770382374525, 42.70261712372303, 35.0667517632246, 36.07932198792696, 39.88824877887964, 42.740508913993835, 36.58740036189556, 38.24377991259098, 41.97032283991575, 41.27949196845293, 35.07478814572096, 37.12202701717615, 37.754991091787815, 39.74622767418623, 41.82693921029568, 37.79126238077879, 41.71545431017876, 40.55408947169781, 38.38333021849394, 36.268237978219986, 38.496607914566994, 39.22815527766943, 35.74974834918976, 36.10651474446058, 42.23136696964502, 41.21979512274265, 37.403883412480354, 37.065912038087845, 38.97352423518896, 39.29493296891451, 37.11321856826544, 36.391944624483585, 36.67099215090275, 38.11994194984436, 37.66245860606432, 36.819628439843655, 37.51773480325937, 39.36339262872934, 36.244092509150505, 35.6999384239316, 41.5471950545907, 37.4032836407423, 35.647157579660416, 37.20417711883783, 38.81410975009203, 36.790831945836544, 35.95795203000307, 38.383021019399166, 36.318608559668064, 34.290602430701256, 42.088876478374004, 53.02397161722183, 43.062406592071056, 46.65026906877756, 39.991531521081924, 38.73767051845789, 36.888075061142445, 35.93656700104475, 37.60438412427902, 41.03210661560297, 34.66880787163973, 44.96041405946016, 37.850722670555115, 36.399113945662975, 37.23111655563116, 33.76605175435543, 34.64715741574764, 37.07655146718025, 37.91859094053507, 38.10035903006792, 34.362245351076126, 34.64720584452152, 37.7163328230381, 36.492026410996914, 36.71274799853563, 37.47966606169939, 43.13588794320822, 42.83510986715555, 35.09286604821682, 39.24855962395668, 35.698615945875645, 36.57706920057535, 35.65142955631018, 41.44357331097126, 45.68744357675314, 47.413830645382404, 38.826375268399715, 42.08541568368673, 39.90555461496115, 36.68255731463432, 37.25917357951403, 38.544222712516785, 36.37542761862278, 36.8051091209054, 36.230950616300106, 36.41775622963905, 36.1250564455986, 35.949026234447956, 35.42518522590399, 36.16793919354677, 34.99423619359732, 36.24959848821163, 35.28312407433987, 35.750080831348896, 35.05591303110123, 35.523644648492336, 35.33901646733284, 35.54139658808708, 35.08329764008522, 36.575183272361755, 35.65902914851904, 35.76938062906265, 35.51675844937563, 40.87660275399685, 36.410827189683914, 38.82445674389601, 45.965767465531826, 43.943618424236774, 42.09860507398844, 36.972230300307274, 36.21205687522888, 36.76222264766693, 36.63301840424538, 37.51984890550375, 37.03251387923956, 42.53672808408737, 37.75174356997013, 35.583571530878544, 36.07514780014753, 38.37542049586773, 41.93749092519283, 36.74064110964537, 36.544013768434525, 38.511390797793865, 41.24607890844345, 35.62629874795675, 45.18774338066578, 39.63471204042435, 50.025167874991894, 48.85190352797508, 53.872463293373585, 55.82321900874376, 47.58128244429827, 42.680452577769756, 35.75820475816727, 34.84881855547428, 37.01538685709238, 42.538147419691086, 42.60679334402084, 38.69703784584999, 44.14127767086029, 36.032683216035366, 35.997651517391205, 38.44569902867079, 42.405773885548115, 36.3283921033144, 37.234872579574585, 38.778637535870075, 38.321441039443016, 36.256649531424046, 36.29119135439396, 38.0271440371871, 40.28985183686018, 37.52867039293051, 36.99332941323519, 39.400747045874596, 43.49941201508045, 36.745877005159855, 36.64596565067768, 38.10385800898075, 42.48173628002405, 35.43019760400057, 37.501160986721516, 39.12053536623716, 41.96548089385033, 35.92313174158335, 36.753540858626366, 41.85936041176319, 37.01182268559933, 36.591554060578346, 40.436869487166405, 38.73288165777922, 39.10456597805023, 37.03631740063429, 41.50092229247093, 36.935821175575256, 37.57243510335684, 36.7200281471014, 34.86187569797039, 35.937280394136906, 37.891777232289314, 37.320150062441826, 38.064547814428806, 38.934958167374134, 38.8891389593482, 36.74825560301542, 36.425686441361904, 36.85061540454626, 54.26958482712507, 46.056244522333145, 56.8380244076252, 49.1036931052804, 53.0397854745388, 43.07607468217611, 41.98783356696367, 33.54002069681883, 34.93123408406973, 39.22316711395979, 41.73158574849367, 34.76801607757807, 38.568771444261074, 41.1792928352952, 37.29603439569473, 40.051921270787716, 40.99629446864128, 36.67415864765644, 42.471266351640224, 41.644105687737465, 35.25881841778755, 35.407572984695435, 36.71364765614271, 36.80182993412018, 38.38566783815622, 35.08431185036898, 35.035849548876286, 41.67551267892122, 41.483321227133274, 37.67405543476343, 35.565330646932125, 37.313614040613174, 37.16044034808874, 37.25562151521444, 34.99623015522957, 35.776153206825256, 41.74781497567892, 36.58960293978453, 41.606731712818146, 40.45237973332405, 37.981689907610416, 36.84087283909321, 38.64401578903198, 37.64520213007927, 36.39353904873133, 35.58809868991375, 35.0961908698082, 37.22588624805212, 35.017349757254124, 36.2932775169611, 36.477736197412014, 34.359884448349476, 34.05960649251938, 37.88804169744253, 36.36617120355368, 37.46517840772867, 35.21064296364784, 34.84364598989487, 35.798707976937294, 36.801847629249096, 36.103153601288795, 37.12525125592947, 36.89936827868223, 36.72925382852554, 35.47591436654329, 37.49240189790726, 36.76072973757982, 35.850392654538155, 34.81866419315338, 36.11620143055916, 34.91200413554907, 35.05739662796259, 34.178391098976135, 34.54322833567858, 36.28780972212553, 33.95809140056372, 35.35281214863062, 36.286141723394394, 35.71035526692867, 35.786766558885574, 34.59147643297911, 35.83087585866451, 36.30452509969473, 36.32401116192341, 36.07185557484627, 41.30036197602749, 35.89914180338383, 52.75833606719971, 52.89630312472582, 43.15698891878128, 44.434214010834694, 35.54237075150013, 34.97138060629368, 36.30890976637602, 34.88888032734394, 37.1644701808691, 35.56390479207039, 38.05301617830992, 35.55372357368469, 39.22313265502453, 35.397532396018505, 36.384803242981434, 35.282766446471214, 37.43041027337313, 36.033935844898224, 37.16116212308407, 36.65218688547611, 38.69308903813362, 37.05386072397232, 36.76576726138592, 37.0483361184597, 41.28742124885321, 36.87641769647598, 38.97488676011562, 37.337020970880985, 37.72862069308758, 38.20293676108122, 38.8009175658226, 39.808171801269054, 46.87695764005184, 37.83712908625603, 39.1464289277792, 35.33230721950531, 34.944853745400906, 37.676298059523106, 40.79595673829317, 36.28550190478563, 35.43930221349001, 36.76316887140274, 40.79356789588928, 39.25047907978296, 46.13429121673107, 39.38077110797167, 41.38284083455801, 36.94728668779135, 34.70033220946789, 35.20139493048191, 37.25413605570793, 37.2034702450037, 37.20261622220278, 41.259102523326874, 36.46483179181814, 36.53878066688776, 38.09536248445511, 36.36604081839323, 36.70745063573122, 36.13155335187912, 40.190404281020164, 37.95691393315792, 41.58374480903149, 38.52144721895456, 36.20869293808937, 36.04143299162388, 36.53405047953129, 37.05800883471966, 44.26870681345463, 42.251949198544025, 40.677040815353394, 42.06685535609722, 37.05956228077412, 36.99957113713026, 41.58428683876991, 42.09848307073116, 37.687793374061584, 43.34658104926348, 37.87920158356428, 35.90784687548876, 37.48317901045084, 36.89130861312151, 40.52376560866833, 39.17692322283983, 40.125615894794464, 39.727688767015934, 42.33194328844547, 41.23427998274565, 39.10673875361681, 36.77082434296608, 36.83645185083151, 34.7848953679204, 34.87286530435085, 35.38615349680185, 35.60316935181618, 43.95019728690386, 40.135083720088005, 37.05805819481611, 40.499310940504074, 35.933252424001694, 37.26412262767553, 37.26127836853266, 34.83149316161871, 38.38383127003908, 39.98585417866707, 35.37902422249317, 36.533065140247345, 42.157452553510666, 37.560886703431606, 35.63937172293663, 49.10021089017391, 52.19934042543173, 52.24971752613783, 45.412033796310425, 49.81670901179314, 39.864521473646164, 38.10014855116606, 34.094199538230896, 34.71483010798693, 36.46794054657221, 36.260562017560005, 35.20460519939661, 37.30441257357597, 37.93824929744005, 33.65920204669237, 36.462824791669846, 43.59608516097069, 38.25014643371105, 37.40717004984617, 36.92683111876249, 38.00930920988321, 35.34295689314604, 34.785106778144836, 35.781740210950375, 35.06617806851864, 35.52796319127083, 35.52737459540367, 36.40221059322357, 37.54355385899544, 40.7232828438282, 36.77137102931738, 36.71561274677515, 36.815643310546875, 37.99451049417257, 36.17160301655531, 35.86120903491974, 35.64547095447779, 35.48778314143419, 34.3004185706377, 34.71068199723959, 36.653488874435425, 35.0209828466177, 35.63595283776522, 34.10120029002428, 35.28593573719263, 33.90891570597887, 35.75666807591915, 35.04027146846056, 33.72893389314413, 34.381830133497715, 35.103555768728256, 34.27121601998806, 33.8893486186862, 34.38998851925135, 34.46855489164591, 34.036802127957344, 34.60906445980072, 37.51769755035639, 34.06161908060312, 35.70221737027168, 33.57373271137476, 36.41215618699789, 33.944944851100445, 36.88035160303116, 33.46376493573189, 35.81430297344923, 34.1133251786232, 36.02615650743246, 35.176265984773636, 38.580579683184624, 40.715934708714485, 33.75942353159189, 35.19683703780174, 34.09901726990938, 35.0918909534812, 34.72988121211529, 35.23490484803915, 34.356086514890194, 36.97885386645794, 35.57457309216261, 38.548083044588566, 36.15327086299658, 35.00818274915218, 38.08657266199589, 37.35160734504461, 36.06951795518398, 35.64621973782778, 36.867144517600536, 37.850349210202694, 36.164483055472374, 35.868178121745586, 42.46971942484379, 35.152786411345005, 35.612693056464195, 38.627819158136845, 36.434256471693516, 36.784213967621326, 37.51427214592695, 42.5477446988225, 40.30107241123915, 35.9036810696125, 33.60424283891916, 38.79460319876671, 36.53748519718647, 35.87225638329983, 35.95434408634901, 34.71820242702961, 36.81458253413439, 38.99407293647528, 40.10550770908594, 37.84406557679176, 36.83581296354532, 41.807716712355614, 39.03873264789581, 37.096123211085796, 38.80272340029478, 45.288849622011185, 42.52167604863644, 53.56727447360754, 41.980234906077385, 43.276953510940075, 41.39223042875528, 34.373500384390354, 35.7521940022707, 39.79261592030525, 37.797833792865276, 33.868806436657906, 42.206572368741035, 40.85133969783783, 35.23618169128895, 36.21019423007965, 38.61488029360771, 35.730188712477684, 35.516269505023956, 42.266868986189365, 42.84508898854256, 34.12383049726486, 35.28335131704807, 37.86382544785738, 36.69014759361744, 38.38376700878143, 34.36891082674265, 34.4085106626153, 39.00107368826866, 36.52945812791586, 36.56947147101164, 35.987683571875095, 38.244957104325294, 35.59147007763386, 38.45297358930111, 38.334463723003864, 37.05931920558214, 37.21287567168474, 36.519947461783886, 35.44292505830526, 35.62628477811813, 38.58881630003452, 38.31499442458153, 33.67064241319895, 34.5618911087513, 35.47222167253494, 34.432126209139824, 35.95072031021118, 36.8676595389843, 35.15217732638121, 35.55296268314123, 34.87494494765997, 35.10913718491793, 34.23789329826832, 34.79671385139227, 36.44348215311766, 36.00488044321537, 36.31655219942331, 34.592147916555405, 35.20783223211765, 35.80264840275049, 36.40640340745449, 35.50258185714483, 35.99230293184519, 34.60289258509874, 35.227347165346146, 35.295634530484676, 35.60651000589132, 34.79502908885479, 34.81139708310366, 34.11671984940767, 35.027218982577324, 35.3985084220767, 35.79223155975342, 34.576267935335636, 38.06030936539173, 35.21185275167227, 38.585906848311424, 34.467616118490696, 37.36659698188305, 34.74755398929119, 37.0086720213294, 36.82324010878801, 36.27556189894676, 36.41613945364952, 39.42184615880251, 36.836556158959866, 42.3462288454175, 37.318904884159565, 35.47434788197279, 42.78001841157675, 35.755143500864506, 34.94568727910519, 36.79295536130667, 34.80824828147888, 39.89613242447376, 35.100423730909824, 39.022606797516346, 45.381355099380016, 40.7300004735589, 42.01673064380884, 40.8140541985631, 35.258859395980835, 37.00251132249832, 38.27416058629751, 35.88271327316761, 36.41118761152029, 42.88642015308142, 46.04226816445589, 44.060103595256805, 35.88057402521372, 35.49461532384157, 33.256860449910164, 36.491298116743565, 34.94877554476261, 38.13539259135723, 42.06364043056965, 35.63604597002268, 37.77786996215582, 37.898327223956585, 36.432355642318726, 35.47564893960953, 42.97482967376709, 36.555102095007896, 36.658371798694134, 34.56361312419176, 42.284742929041386, 38.92534226179123, 34.926860593259335, 36.66946571320295, 38.68560865521431, 36.61675192415714, 36.501314491033554, 38.80114667117596, 41.76188167184591, 35.44509317725897, 33.401912078261375, 35.23145988583565, 41.58178623765707, 35.54101847112179, 33.9147699996829, 38.85145951062441, 41.928923688828945, 37.62552887201309, 37.48571779578924, 35.055468790233135, 36.28447186201811, 38.24044298380613, 38.33519667387009, 38.19585684686899, 38.34845405071974, 41.96773376315832, 35.90518143028021, 33.968872390687466, 40.75831826776266, 39.79083802551031, 39.09403458237648, 42.76368673890829, 37.78249304741621, 36.527800373733044, 37.42167353630066, 34.73748825490475, 34.207639284431934, 36.668915301561356, 38.19967433810234, 38.10855746269226, 34.00206658989191, 36.06302663683891, 37.51285746693611, 40.12093506753445, 37.52931393682957, 34.76705960929394, 36.31707839667797, 41.6491124778986, 38.70084322988987, 34.648509696125984, 37.42960374802351, 37.48874459415674, 35.802255384624004, 35.40368936955929, 41.11007507890463, 37.98187244683504, 42.18458104878664, 38.687451742589474, 37.12774068117142, 38.512698374688625, 35.24737246334553, 35.489192232489586, 35.81871930509806, 36.41805611550808, 36.11849434673786, 36.14942077547312, 35.737184807658195, 36.38257645070553, 36.280288361012936, 34.323795698583126, 36.80003900080919, 39.44343701004982, 38.131168112158775, 36.38243768364191, 36.519608460366726, 36.94331832230091, 35.477785393595695, 34.06831901520491, 34.86279956996441, 34.951226785779, 33.69311522692442, 33.61161891371012, 33.961630426347256, 33.45147706568241, 34.60192773491144, 34.754760563373566, 34.59872771054506, 35.26157047599554, 34.44553539156914, 34.386953338980675, 33.82282890379429, 34.41653773188591, 36.380949430167675, 34.601825289428234, 34.711617045104504, 36.51969786733389, 34.86347198486328, 33.35540369153023, 34.66455452144146, 33.77043269574642, 34.8900081589818, 34.595618955791, 36.57782822847366, 35.21175030618906, 34.14696082472801, 35.11226549744606, 34.17359944432974, 34.795633517205715, 35.09368933737278, 35.549551248550415, 33.57334341853857, 35.69875471293926, 36.09813656657934, 36.399977281689644, 36.3333523273468, 36.91100049763918, 36.80728003382683, 36.2051036208868, 37.78662346303463, 39.87110685557127, 41.506784968078136, 38.18540368229151, 36.924573592841625, 37.336571142077446, 38.84019888937473, 36.65142133831978, 37.19243314117193, 36.597663536667824, 42.71870944648981, 38.32205105572939, 36.156061105430126, 37.25991304963827, 37.10301220417023, 37.20318991690874, 36.80369630455971, 35.73702834546566, 43.952422216534615, 42.1786205843091, 37.63905726373196, 36.226749420166016, 35.62409710139036, 36.14801447838545, 39.13641721010208, 37.70865499973297, 37.04249858856201, 35.265401005744934, 41.13990068435669, 37.165356799960136, 36.858790554106236, 35.956221632659435, 44.37804687768221, 43.40791329741478, 37.30435483157635, 37.36832458525896, 36.9916595518589, 34.60288606584072, 39.07763585448265, 37.68098261207342, 35.390143282711506, 38.343410938978195, 38.47116511315107, 44.512031599879265, 35.15977784991264, 35.489137284457684, 41.31328593939543, 35.05127131938934, 38.63829933106899, 42.29073226451874, 33.92220288515091, 36.44638042896986, 38.73855713754892, 42.075940407812595, 37.67832089215517, 43.5284785926342, 41.52868781238794, 33.99325534701347, 38.26257586479187, 35.92222090810537, 44.224304147064686, 42.23829600960016, 41.40165261924267, 38.09806611388922, 41.78679082542658, 35.95074638724327, 34.071735106408596, 38.49013242870569, 38.283947855234146, 38.720471784472466, 36.46821901202202, 38.21880277246237, 41.685931384563446, 37.7514474093914, 35.39386764168739, 41.705588810145855, 39.74541462957859, 34.252568148076534, 34.37398001551628, 38.14547974616289, 36.839463748037815, 36.897958256304264, 38.77591248601675, 38.15900348126888, 37.76232618838549, 36.54891438782215, 36.001503467559814, 37.75790985673666, 36.444876343011856, 36.91069968044758, 35.165512934327126, 42.79062058776617, 40.868562646210194, 36.32420115172863, 36.20794042944908, 37.04551514238119, 34.05468724668026, 34.270442090928555, 37.497127428650856, 37.267498672008514, 36.31977457553148, 34.959676675498486, 38.07676210999489, 36.44822631031275, 35.68090219050646, 37.930901162326336, 35.09065788239241, 37.85321582108736, 38.183003664016724, 37.65222895890474, 37.92367223650217, 37.7308614552021, 35.85754334926605, 37.88079787045717, 42.37842094153166, 35.39961762726307, 36.59874852746725, 36.07221879065037, 33.82888063788414, 34.989998675882816, 34.7939832136035, 36.147696897387505, 36.23423911631107, 36.524685099720955, 37.063381634652615, 33.96966401487589, 36.13055497407913, 34.42240320146084, 35.6886750087142, 37.87996619939804, 36.25369817018509, 35.28235852718353, 36.65934782475233, 35.21130606532097, 36.76729090511799, 34.51028652489185, 38.50192856043577, 37.44222968816757, 45.34594900906086, 38.19493483752012, 39.476120844483376, 35.889714024960995, 35.2676585316658, 35.75680125504732, 36.17895394563675, 36.08637675642967, 37.78532613068819, 36.49603109806776, 36.64050996303558, 42.316838167607784, 42.000764049589634, 44.34042237699032, 37.85325866192579, 38.50053809583187, 42.357396334409714, 45.415847562253475, 36.84271685779095, 35.76061502099037, 36.40813659876585, 35.48837173730135, 38.85077312588692, 36.13565210253, 37.72117476910353, 42.19964053481817, 44.64634042233229, 36.62531543523073, 42.03128069639206, 38.21474500000477, 35.83574015647173, 38.83427567780018, 38.37260045111179, 37.04216703772545, 41.4336072281003, 41.81563574820757, 37.3530900105834, 36.77820693701506, 44.23788469284773, 42.67857503145933, 37.1746439486742, 38.336293771862984, 42.04163793474436, 37.436243146657944, 35.33704113215208, 36.42277047038078, 36.24406922608614, 38.69254142045975, 37.09392808377743, 36.6592425853014, 38.05593308061361, 39.397766813635826, 36.27955541014671, 36.030991934239864, 38.8574218377471, 41.28910880535841, 36.09914518892765, 49.30425342172384, 39.99632690101862, 43.822748586535454, 35.60528066009283, 34.26473867148161, 45.40478065609932, 37.86146640777588, 42.20407176762819, 44.37533859163523, 34.176332876086235, 37.01916616410017, 37.576453760266304, 36.5565475076437, 42.540498077869415, 42.01037064194679, 37.222836166620255, 35.009387880563736, 38.58495969325304, 37.36664727330208, 35.09117569774389, 37.485078908503056, 38.87150716036558, 37.111314944922924, 37.425776943564415, 37.02999651432037, 38.1750063970685, 38.231140933930874, 35.456365905702114, 38.9675609767437, 40.23607540875673, 36.725287325680256, 36.14833019673824, 41.735902428627014, 38.31993788480759, 35.248261876404285, 35.057985223829746, 38.11629116535187, 38.5164450854063, 34.59522593766451, 35.68345494568348, 42.04224236309528, 39.182052947580814, 35.69660149514675, 43.01392659544945, 40.06160423159599, 39.86035846173763, 36.29255015403032, 42.80208423733711, 37.44637034833431, 34.45037454366684, 35.553619265556335, 35.20630020648241, 36.79034020751715, 37.06846572458744, 37.73036785423756, 38.03123068064451, 37.05320227891207, 40.060775354504585, 40.43667670339346, 34.80909299105406, 36.90496273338795, 36.85656189918518, 34.13937706500292, 34.88426562398672, 44.364191591739655, 38.187213242053986, 35.622513853013515, 36.875017918646336, 34.0074822306633, 37.71852143108845, 35.926018841564655, 36.24447248876095, 36.629002541303635, 34.63304694741964, 35.0102698430419, 36.315602250397205, 35.58790124952793, 36.36796399950981, 35.62408220022917, 35.06517969071865, 35.503631457686424, 34.88758206367493, 35.05620639771223, 35.443173721432686, 35.7122840359807, 35.02271696925163, 34.27017945796251, 33.71648583561182, 34.253369085490704, 36.35730408132076, 36.64787299931049, 35.40399298071861, 35.919700749218464, 35.76076868921518, 36.36141959577799, 34.2292757704854, 35.18832288682461, 36.11345589160919, 36.37581318616867, 35.97336169332266, 37.3535780236125, 38.81938382983208, 42.72827133536339, 35.432140342891216, 37.259616889059544, 35.510667599737644, 37.511167116463184, 35.85640713572502, 37.57820278406143, 35.477058961987495, 38.375306874513626, 34.81793776154518, 37.9283269867301, 35.009099170565605, 39.415315724909306, 34.442923963069916, 38.720290176570415, 37.21271641552448, 40.96025973558426, 40.06645921617746, 36.455316469073296, 37.8135247156024, 37.34051715582609, 38.37156388908625, 38.519821129739285, 36.91239282488823, 40.381528437137604, 37.92838007211685, 37.87437453866005, 36.670977249741554, 41.74006450921297, 40.976119227707386, 37.50517498701811, 36.7328692227602, 40.27440771460533, 37.229699082672596, 49.627126194536686, 43.78035571426153, 53.838057443499565, 47.16233350336552, 48.13837539404631, 41.41111392527819, 38.28031849116087, 39.01651408523321, 36.161141470074654, 37.30655089020729, 45.37477996200323, 44.30864937603474, 38.91077823936939, 38.74716255813837, 38.57166972011328, 35.632955841720104, 40.840606205165386, 42.26065706461668, 52.66775656491518, 43.90029422938824, 44.900765642523766, 43.52864436805248, 36.18950769305229, 34.60947796702385, 33.99672731757164, 38.497607223689556, 36.750588566064835, 37.122310139238834, 45.619310811161995, 49.738312140107155, 44.59646716713905, 45.36385275423527, 36.56377270817757, 35.502768121659756, 36.4975044503808, 34.80864595621824, 38.270425982773304, 38.58158364892006, 37.519847974181175, 36.490161903202534, 35.93921847641468, 38.34418673068285, 36.34756524115801, 35.325707867741585, 38.82798179984093, 41.73851851373911, 40.65985977649689, 38.020309060812, 41.16545058786869, 33.56170188635588, 33.77786185592413, 37.28818241506815, 38.007382303476334, 38.83737977594137, 36.814999766647816, 41.84744693338871, 39.6495359018445, 43.1120190769434, 39.48153555393219, 35.95011401921511, 34.00387056171894, 38.71589154005051, 37.785179913043976, 35.08324548602104, 41.67682770639658, 41.87722597271204, 34.35000404715538, 36.41640394926071, 41.70344490557909, 40.689317509531975, 43.66711247712374, 36.90329007804394, 42.19794645905495, 38.484049029648304, 34.039197489619255, 37.04525623470545, 42.28622280061245, 37.1632007881999, 36.465334706008434, 35.86666937917471, 36.31836175918579, 38.072929717600346, 35.91336775571108, 38.412985391914845, 41.56453441828489, 38.90856262296438, 37.91417088359594, 40.72888940572739, 34.94519740343094, 33.613571897149086, 36.70234605669975, 35.10793298482895, 38.3530305698514, 35.906814970076084, 35.85517220199108, 38.33836875855923, 36.32525261491537, 34.31434277445078, 39.626386016607285, 40.10798130184412, 35.62468197196722, 38.157898001372814, 36.48955188691616, 34.990149550139904, 37.30663191527128, 34.78012699633837, 36.62247769534588, 38.398570381104946, 35.497345961630344, 36.85502242296934, 42.19209775328636, 39.92041479796171, 42.084221728146076, 35.65542586147785, 39.44992646574974, 37.9160949960351, 35.796008072793484, 35.841869190335274, 39.00089953094721, 36.69582773000002, 35.315888933837414, 37.33628988265991, 35.34000366926193, 35.407885909080505, 34.49587896466255, 34.418487921357155, 34.68634560704231, 34.76205002516508, 35.62573716044426, 38.07821497321129, 43.00264082849026, 42.89608169347048, 38.502929732203484, 38.652196526527405, 35.35739146173, 35.29869019985199, 34.79322977364063, 39.62244000285864, 37.81384788453579, 48.66501875221729, 36.43007576465607, 42.21520386636257, 36.10305767506361, 37.603444419801235, 34.421566873788834, 35.29542963951826, 34.76124536246061, 36.4686232060194, 34.57235172390938, 35.65778210759163, 34.78432260453701, 35.81293672323227, 34.460817463696, 35.664983093738556, 35.26678681373596, 35.40141973644495, 36.0416816547513, 36.07254195958376, 35.84097418934107, 36.01447306573391, 36.160385236144066, 35.169655457139015, 34.53997150063515, 35.43482534587383, 37.465253844857216, 43.637930415570736, 43.07680297642946, 38.612520322203636, 36.13637015223503, 36.50667518377304, 42.74477902799845, 38.4147297590971, 36.30336280912161, 38.95385190844536, 42.04333666712046, 40.18247593194246, 36.747291684150696, 36.25677525997162, 38.59194740653038, 35.60111951082945, 37.72078175097704, 39.924983866512775, 38.63370884209871, 36.67062986642122, 37.27598022669554, 42.08230972290039, 37.87591494619846, 35.39644740521908, 35.59289872646332, 37.80767600983381, 42.310879565775394, 41.73831827938557, 40.234945714473724, 35.577647387981415, 34.67742260545492, 38.32836728543043, 39.19891268014908, 36.10770683735609, 36.1008383333683, 42.475588619709015, 38.928973488509655, 35.566553473472595, 37.39489987492561, 41.62312112748623, 42.17447340488434, 39.94942083954811, 33.79904571920633, 34.32645834982395, 38.78686763346195, 38.562060333788395, 43.87678299099207, 44.4851778447628, 45.560447499156, 36.4272752776742, 42.103041894733906, 35.66098492592573, 36.60509828478098, 36.062296479940414, 37.635551765561104, 37.85262908786535, 42.288792319595814, 41.884525679051876, 36.25565581023693, 37.97278739511967, 37.015896290540695, 32.98118431121111, 37.20350004732609, 43.093801476061344, 37.667385302484035, 39.673333056271076, 41.57825652509928, 42.26021096110344, 37.58750669658184, 35.78332718461752, 42.539944872260094, 48.941791988909245, 43.502822518348694, 42.44178347289562, 35.57232953608036, 34.67696439474821, 35.17680708318949, 34.64842028915882, 35.32141726464033, 33.002388663589954, 34.76064559072256, 34.383066929876804, 36.02983523160219, 40.693728253245354, 42.811643332242966, 37.69534174352884, 37.57232706993818, 37.11394779384136, 32.70277939736843, 32.4313510209322, 34.4487726688385, 35.48578452318907, 35.680743865668774, 35.113695077598095, 36.201491951942444, 36.05595510452986, 34.77480076253414, 36.442712880671024, 36.146034486591816, 35.51049251109362, 35.82681901752949, 35.73167230933905, 35.82917992025614, 36.16096079349518, 35.02984903752804, 35.194870084524155, 35.53704172372818, 34.591169096529484, 34.778473898768425, 35.34934110939503, 34.47853587567806, 34.00696348398924, 34.35264993458986, 38.209060207009315, 34.68608949333429, 36.89887560904026, 35.67980136722326, 37.196921184659004, 39.038279093801975, 37.64480445533991, 45.52842769771814, 36.98068391531706, 41.78026504814625, 33.485724590718746, 37.584894336760044, 34.463318064808846, 37.63392847031355, 34.04923900961876, 39.005265571177006, 34.59681198000908, 39.46029022336006, 35.600628703832626, 41.42638295888901, 35.46286281198263, 38.35373651236296, 35.72568390518427, 33.88400375843048, 44.42261904478073, 49.530806951224804, 47.294859774410725, 44.17851474136114, 39.02724664658308, 35.19333899021149, 36.74493730068207, 34.476472064852715, 36.39209922403097, 35.83288099616766, 37.259966135025024, 36.603600718081, 43.12526900321245, 37.95772138983011, 35.81428900361061, 34.661308862268925, 36.58479359000921, 36.7717994377017, 36.96189634501934, 36.81666310876608, 36.82525083422661, 38.9179028570652, 37.27574646472931, 35.95911059528589, 42.49509144574404, 37.22674306482077, 36.3974217325449, 36.54429782181978, 38.590616546571255, 36.88838426023722, 39.03848025947809, 48.58084302395582, 39.081428200006485, 44.06353924423456, 36.61296144127846, 43.12518518418074, 33.60534738749266, 39.91455212235451, 34.49884243309498, 36.470621824264526, 37.6246701925993, 37.191455252468586, 36.03321220725775, 36.6000896319747, 38.379967212677, 39.11453206092119, 46.94396909326315, 38.051873445510864, 39.76637125015259, 43.262362480163574, 40.25629349052906, 35.90862080454826, 35.149126313626766, 41.68521612882614, 39.34513870626688, 37.66176477074623, 37.30301931500435, 42.15795174241066, 40.31942505389452, 38.90528902411461, 38.494438864290714, 38.94862439483404, 40.962315164506435, 43.40068157762289, 36.381970159709454, 36.776394583284855, 40.28259217739105, 34.591312520205975, 37.30290476232767, 42.40554105490446, 39.77767191827297, 41.661146096885204, 36.07803676277399, 36.473301239311695, 41.54560435563326, 37.42966242134571, 35.154868848621845, 37.366860546171665, 37.06521634012461, 43.476635590195656, 39.93106819689274, 36.94816306233406, 33.40453468263149, 42.10690129548311, 39.69675116240978, 34.85605586320162, 39.429547265172005, 37.2040718793869, 36.25088278204203, 37.672518752515316, 37.23572567105293, 41.999831795692444, 42.691982351243496, 39.98797666281462, 35.48312373459339, 37.81630005687475, 35.92338040471077, 35.25172173976898, 38.60031347721815, 37.230730056762695, 34.934367053210735, 37.53882832825184, 36.07749566435814, 37.881024181842804, 38.309505209326744, 35.498895682394505, 34.317330457270145, 38.22031430900097, 40.55369179695845, 43.701802380383015, 39.32974487543106, 41.48351587355137, 34.72467325627804, 36.71739250421524, 40.55264126509428, 33.75312499701977, 44.217899441719055, 43.89845672994852, 40.943725034594536, 37.964106537401676, 35.01731902360916, 35.486635752022266, 36.065381951630116, 37.63495106250048, 42.3301886767149, 37.762509658932686, 37.1487969532609, 36.42243426293135, 35.98945029079914, 37.13800851255655, 35.88286601006985, 34.21255853027105, 36.31932940334082, 35.35566106438637, 34.26381014287472, 35.80756485462189, 34.24984589219093, 35.82953009754419, 35.902428440749645, 35.53395066410303, 35.24656593799591, 35.26057954877615, 35.809860564768314, 35.589976236224174, 34.82556715607643, 35.53143050521612, 37.02171798795462, 37.928770296275616, 38.47657609730959, 38.64606935530901, 45.45010253787041, 36.70806810259819, 38.86106237769127, 35.183632746338844, 39.15012162178755, 35.87076906114817, 38.15714083611965, 36.752164363861084, 37.371233105659485, 37.80958894640207, 38.325194269418716, 37.857526913285255, 36.78805101662874, 39.55777548253536, 36.226908676326275, 38.571326062083244, 38.326322101056576, 41.013496927917004, 38.51832915097475, 45.797744765877724, 37.10465133190155, 40.91416206210852, 35.16076412051916, 38.09771221131086, 37.46996447443962, 44.242129661142826, 37.287029437720776, 41.58590082079172, 37.93446905910969, 36.386857740581036, 37.43266128003597, 45.049313455820084, 40.431770496070385, 49.88216143101454, 42.299794033169746, 37.40978427231312, 35.599445924162865, 41.356343775987625, 35.41658818721771, 40.52693024277687, 37.45455667376518, 38.341145031154156, 36.92801296710968, 41.47123917937279, 36.74113843590021, 41.437139734625816, 40.753912180662155, 34.840294159948826, 36.541529931128025, 40.26872385293245, 46.51184566318989, 42.55524557083845, 39.88461196422577, 43.88519935309887, 35.658142529428005, 36.49317845702171, 45.560204423964024, 36.91790904849768, 42.6951888948679, 49.711315892636776, 52.72714421</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mu (qps)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cv</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t># requests</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Latency Constraint (ms)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Planner</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estimated Latency (ms)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Ingest mu Observed (qps)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Throughput (qps)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>p95 (ms)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>p99 (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>SimulatedAnnealing</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>71.74977540969849</v>
+      </c>
+      <c r="H2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="J2" t="n">
+        <v>98.76414033046157</v>
+      </c>
+      <c r="K2" t="n">
+        <v>248.5961322810154</v>
+      </c>
+      <c r="L2" t="n">
+        <v>44.60133453831076</v>
+      </c>
+      <c r="M2" t="n">
+        <v>54.174537230283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mu (qps)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cv</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t># requests</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Latency Constraint (ms)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Planner</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estimated Latency (ms)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Latency (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>SimulatedAnnealing</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>71.74977540969849</v>
+      </c>
+      <c r="H2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>[68.35087947547436, 57.64685571193695, 60.64381171017885, 78.34525872021914, 83.04187469184399, 95.98721470683813, 86.12491562962532, 82.80190639197826, 75.64895134419203, 72.00647983700037, 62.730069272220135, 58.9105598628521, 48.96599147468805, 41.1275802180171, 37.99539525061846, 34.92119535803795, 37.16700151562691, 38.75986114144325, 36.7805203422904, 41.52652435004711, 36.48756816983223, 40.87043460458517, 35.62030475586653, 34.80731137096882, 35.911403596401215, 35.45122966170311, 34.516749903559685, 34.05838832259178, 34.917877055704594, 35.50196252763271, 34.86997727304697, 35.285813733935356, 35.6956347823143, 35.515434108674526, 35.60853190720081, 35.63164174556732, 34.94166396558285, 37.53244411200285, 38.82682789117098, 33.96463580429554, 37.32582274824381, 34.92231573909521, 36.047568544745445, 39.17049616575241, 42.79862344264984, 33.81606377661228, 38.784909062087536, 33.71695429086685, 33.370355144143105, 31.895280815660954, 38.25432900339365, 40.25760944932699, 33.606759272515774, 33.79807900637388, 34.903429448604584, 34.22904759645462, 36.69045586138964, 35.80524493008852, 40.40436539798975, 35.053384490311146, 38.630747236311436, 38.69597241282463, 45.69024499505758, 37.551562301814556, 40.14613572508097, 36.72222327440977, 42.264893651008606, 38.6370038613677, 37.97749150544405, 36.14754043519497, 41.26534052193165, 42.81034041196108, 36.26294154673815, 38.659379817545414, 42.13862121105194, 36.202844232320786, 42.3685684800148, 39.516592398285866, 37.140135653316975, 35.92941164970398, 42.059434577822685, 42.53108520060778, 37.313150241971016, 36.25539690256119, 43.42174343764782, 38.11286296695471, 38.16654533147812, 42.30303876101971, 36.987063474953175, 36.58390790224075, 45.022246427834034, 38.645390421152115, 39.01771269738674, 36.28909774124622, 34.66799110174179, 39.57035765051842, 41.569764725863934, 37.443507462739944, 37.79043164104223, 43.67149341851473, 39.57409504801035, 35.970267839729786, 37.5455254688859, 36.96282301098108, 36.70219983905554, 41.46043583750725, 38.69224339723587, 36.26374900341034, 41.924319230020046, 40.23892432451248, 36.355179734528065, 38.2800567895174, 44.29171234369278, 39.306389167904854, 36.7205860093236, 37.65830956399441, 41.97131469845772, 42.51105524599552, 35.040320828557014, 37.58247848600149, 38.57004176825285, 33.8858375325799, 34.84387416392565, 35.70618573576212, 43.820975348353386, 44.105418026447296, 39.293996058404446, 34.52201932668686, 36.85679752379656, 42.053365148603916, 39.53578136861324, 37.24236600100994, 42.97348763793707, 35.19800491631031, 35.052476450800896, 38.02639152854681, 36.64201404899359, 32.13805239647627, 32.124193385243416, 34.243022091686726, 37.068513222038746, 36.53653711080551, 36.33286710828543, 35.92361882328987, 35.004111006855965, 36.6502245888114, 37.180161103606224, 38.66011090576649, 36.11941449344158, 35.59686802327633, 35.78041587024927, 38.020020350813866, 37.474250420928, 36.204587668180466, 38.397831842303276, 46.83383647352457, 44.001255184412, 36.7343258112669, 37.27393038570881, 34.15250591933727, 35.65097786486149, 36.00219450891018, 34.98026542365551, 36.62767447531223, 34.826962277293205, 36.10540647059679, 37.05715108662844, 35.47901753336191, 35.17374210059643, 35.32419539988041, 35.671004094183445, 36.88717260956764, 36.48592997342348, 35.931178368628025, 35.9571622684598, 35.16201488673687, 35.740116611123085, 35.06102040410042, 36.31162736564875, 35.529705695807934, 35.90357583016157, 36.53392381966114, 35.594481974840164, 35.81508155912161, 34.704795107245445, 35.43515503406525, 34.62296351790428, 34.915074706077576, 36.84579115360975, 35.30093375593424, 36.76613140851259, 35.13099253177643, 36.33461240679026, 34.75233633071184, 35.64990404993296, 35.715293139219284, 35.131679847836494, 35.06545536220074, 34.90576799958944, 35.087961703538895, 35.30910238623619, 36.4726772531867, 34.79824122041464, 35.946269519627094, 34.4411376863718, 35.53017694503069, 35.496399737894535, 35.37194151431322, 34.48616433888674, 35.610899329185486, 34.842501394450665, 35.73057893663645, 34.902689047157764, 35.732701420784, 35.24342551827431, 35.52120923995972, 34.480005502700806, 42.077742516994476, 34.91270635277033, 33.59901811927557, 34.14535243064165, 34.91331450641155, 36.62413731217384, 36.1328786239028, 34.5250116661191, 35.36460921168327, 33.43384154140949, 35.50356067717075, 33.30204822123051, 34.7105972468853, 34.435661509633064, 34.11875572055578, 33.36823172867298, 33.794849179685116, 33.78049563616514, 34.89156439900398, 33.75695552676916, 34.30524654686451, 34.91466213017702, 35.975173115730286, 34.491220489144325, 41.737367399036884, 45.68342585116625, 38.91056217253208, 49.74226746708155, 37.485698238015175, 37.73861937224865, 35.355561412870884, 39.71088584512472, 35.97681038081646, 44.08972430974245, 37.48183511197567, 45.74467521160841, 53.256191313266754, 41.291793808341026, 48.37803170084953, 37.69513685256243, 37.68446855247021, 36.51978448033333, 34.95124727487564, 37.642757408320904, 37.220087833702564, 39.781101047992706, 41.95237997919321, 37.14791312813759, 36.991278640925884, 41.55142139643431, 38.30753918737173, 36.8873942643404, 37.80735097825527, 38.418788462877274, 45.03029678016901, 35.76318267732859, 36.75948828458786, 42.01393015682697, 33.784727565944195, 38.78789395093918, 37.3262744396925, 35.331809893250465, 34.211840480566025, 35.53117159754038, 34.9532226100564, 32.97576121985912, 34.0654281899333, 37.94491570442915, 38.156199268996716, 36.41447890549898, 36.7258545011282, 42.043677531182766, 42.66358632594347, 42.465463280677795, 36.25525161623955, 38.31652831286192, 39.61717803031206, 36.04960162192583, 36.477710120379925, 43.710462749004364, 41.47315677255392, 38.01399376243353, 38.29210717231035, 41.31838958710432, 34.076628275215626, 34.69358291476965, 42.6926976069808, 37.00785245746374, 40.415587835013866, 43.97315625101328, 46.83456663042307, 37.974598817527294, 41.50662571191788, 34.64682027697563, 34.927393309772015, 42.371767573058605, 38.79467025399208, 40.179671719670296, 38.38264476507902, 33.45519304275513, 35.704147070646286, 35.27440130710602, 39.93344306945801, 45.470734126865864, 37.115984596312046, 42.47321467846632, 42.72010922431946, 36.85884829610586, 34.59807578474283, 34.78718642145395, 42.00415965169668, 38.067249581217766, 39.82601407915354, 34.972009249031544, 37.47528325766325, 39.11925386637449, 38.80493901669979, 38.68361655622721, 35.14700569212437, 35.949849523603916, 34.1828390955925, 35.444057546555996, 36.23097017407417, 37.730125710368156, 34.60335545241833, 34.34308525174856, 40.14389589428902, 36.31489258259535, 39.87741004675627, 37.648933939635754, 37.18357905745506, 35.23906692862511, 37.41238173097372, 37.8013476729393, 44.845941476523876, 35.90264916419983, 37.785627879202366, 36.03009507060051, 33.552306704223156, 37.90947701781988, 37.23764047026634, 34.99255329370499, 36.73342987895012, 37.73838188499212, 36.60319186747074, 37.31135651469231, 34.51612126082182, 34.84410420060158, 36.70462965965271, 35.857003182172775, 35.79016216099262, 35.18029674887657, 41.90298542380333, 47.26643580943346, 42.31792129576206, 42.001618072390556, 38.16080931574106, 38.32695819437504, 36.68195568025112, 32.99207892268896, 34.64388567954302, 33.218830823898315, 33.87253824621439, 32.05863758921623, 34.569055773317814, 38.19124586880207, 34.85890757292509, 37.6307163387537, 34.26085598766804, 37.562862038612366, 34.68696400523186, 35.47456953674555, 35.52545979619026, 35.915037617087364, 35.84583196789026, 35.910049453377724, 35.10836232453585, 35.350628197193146, 35.16938257962465, 34.84956827014685, 35.313903354108334, 33.79554580897093, 35.24181246757507, 35.9859187155962, 35.056871362030506, 35.97262687981129, 34.5604382455349, 35.48222314566374, 36.25685628503561, 35.50795838236809, 35.31353361904621, 35.510105080902576, 36.003999412059784, 35.493532195687294, 36.08526010066271, 38.22393715381622, 48.342800699174404, 42.15450491756201, 52.62682493776083, 43.74747071415186, 40.85948970168829, 51.91319063305855, 49.11343473941088, 42.157309129834175, 45.48176843672991, 40.758284740149975, 35.33404599875212, 36.8045074865222, 34.680450335145, 36.347425542771816, 36.40578035265207, 35.93533206731081, 37.06528339534998, 39.66926131397486, 37.312679924070835, 40.62694497406483, 36.96181531995535, 41.98450408875942, 42.38815326243639, 38.411869667470455, 36.47041693329811, 38.01855444908142, 39.01553153991699, 40.14984145760536, 35.72687227278948, 35.83987057209015, 37.61677443981171, 36.92372236400843, 34.9187022075057, 36.78505215793848, 37.31572348624468, 35.77038086950779, 36.08143050223589, 37.78122831135988, 36.50992177426815, 35.78175324946642, 38.14382944256067, 40.99571704864502, 36.898075602948666, 34.043614752590656, 37.88334131240845, 35.69039609283209, 36.688548512756824, 37.33235411345959, 36.2564492970705, 35.88989283889532, 35.88353842496872, 36.40818875283003, 37.59553097188473, 36.49011719971895, 35.64772102981806, 35.629935562610626, 39.01733737438917, 37.95075137168169, 37.25497703999281, 35.23088525980711, 38.7406162917614, 39.12384808063507, 35.44258698821068, 35.82744486629963, 39.679416455328465, 38.92275970429182, 37.788115441799164, 40.79961683601141, 36.96056175976992, 34.923589788377285, 34.87961366772652, 36.3943949341774, 37.14001923799515, 37.61906735599041, 34.49168987572193, 34.00340862572193, 38.49566075950861, 39.69752322882414, 34.28105730563402, 35.14935169368982, 38.76040689647198, 37.24186960607767, 37.26615943014622, 36.64563037455082, 37.141213193535805, 34.82573479413986, 36.03283129632473, 39.47664611041546, 41.30412172526121, 53.199886344373226, 43.50254498422146, 44.069879688322544, 38.428294472396374, 36.00536473095417, 37.07147762179375, 32.7812759205699, 33.36869180202484, 37.19013091176748, 38.407910615205765, 41.00803192704916, 32.85400103777647, 33.76194555312395, 36.45822871476412, 38.02237845957279, 37.14666049927473, 39.39226362854242, 38.10053411871195, 37.6290138810873, 35.51650978624821, 36.06341779232025, 35.781871527433395, 35.979350097477436, 36.92212142050266, 34.81285832822323, 35.9687115997076, 35.63504759222269, 34.0972738340497, 35.787422209978104, 36.948916502296925, 37.42389567196369, 34.53307319432497, 36.14242747426033, 36.23922821134329, 35.87346989661455, 34.92090664803982, 36.0721368342638, 35.533422604203224, 34.84291397035122, 35.47754045575857, 34.78146344423294, 36.089302971959114, 40.787105448544025, 37.53684274852276, 38.68246078491211, 41.702982038259506, 41.57646652311087, 37.22826577723026, 36.702413111925125, 36.19896061718464, 36.08309756964445, 35.622524097561836, 35.45919805765152, 35.040280781686306, 35.04115156829357, 47.12662007659674, 41.34450200945139, 38.86127378791571, 37.198944948613644, 37.190658040344715, 35.766614601016045, 38.35427016019821, 35.42645834386349, 37.69893106073141, 35.63597798347473, 37.439869716763496, 35.92989407479763, 37.36366517841816, 36.19324788451195, 36.769118160009384, 36.35776415467262, 40.15297535806894, 42.14875213801861, 38.33384905010462, 36.16280201822519, 37.598997354507446, 36.25860717147589, 37.802981212735176, 36.62395104765892, 37.653762847185135, 40.869295597076416, 38.61300926655531, 36.20406426489353, 41.84237960726023, 40.54808244109154, 35.87781358510256, 35.19631549715996, 38.657340221107006, 36.44505422562361, 35.68024467676878, 37.139385007321835, 39.34089466929436, 43.952956795692444, 37.848787382245064, 35.69227922707796, 40.845150128006935, 42.90858469903469, 36.1262746155262, 38.09432964771986, 38.36141899228096, 35.759556107223034, 36.47321090102196, 36.744448356330395, 38.73825818300247, 42.1100128442049, 35.4749346151948, 35.69074347615242, 39.5981976762414, 38.73835317790508, 38.42137660831213, 35.138619132339954, 35.860137082636356, 37.98320144414902, 36.903535947203636, 35.8683280646801, 37.890082225203514, 39.14661519229412, 45.3658951446414, 58.19650646299124, 49.47386682033539, 46.118251979351044, 42.01057367026806, 42.20488667488098, 36.81617230176926, 38.124035112559795, 40.5276520177722, 36.17668151855469, 42.968438006937504, 41.29755590111017, 34.050348214805126, 35.73957830667496, 37.83826343715191, 38.120780140161514, 41.595530696213245, 37.577591836452484, 38.28073758631945, 41.51309560984373, 36.08858585357666, 35.718413069844246, 42.39235073328018, 36.96299344301224, 36.1824119463563, 44.70928944647312, 49.30694866925478, 42.903379537165165, 45.472756028175354, 37.24375553429127, 37.09560539573431, 37.603299133479595, 35.852763801813126, 34.04877334833145, 32.86839369684458, 38.961743004620075, 42.58704651147127, 40.39797838777304, 38.677637465298176, 41.69135354459286, 35.62335483729839, 41.35820176452398, 36.80125065147877, 38.255758583545685, 40.42874090373516, 36.92514728754759, 33.6371548473835, 35.40677856653929, 36.242080852389336, 35.619841888546944, 35.013819113373756, 38.596559315919876, 36.924637854099274, 37.69276663661003, 36.03232093155384, 36.26070823520422, 35.90960428118706, 36.60413157194853, 37.19226364046335, 36.631652154028416, 36.742059513926506, 36.423753015697, 34.401725977659225, 35.42017098516226, 35.133132711052895, 35.85853707045317, 35.96329875290394, 36.594875156879425, 34.83495023101568, 36.07628587633371, 37.03054506331682, 36.45540401339531, 35.52106115967035, 35.371492616832256, 38.12114614993334, 34.808214753866196, 34.33816321194172, 35.453593358397484, 38.01940940320492, 35.18518898636103, 34.830888733267784, 36.23142931610346, 35.41950322687626, 36.0278207808733, 35.81997752189636, 37.10720594972372, 36.89154423773289, 33.917078748345375, 36.391472443938255, 35.639915615320206, 35.985066555440426, 35.10363306850195, 35.19056178629398, 34.73981004208326, 35.60780547559261, 45.34682258963585, 50.92778895050287, 45.53294274955988, 44.58524100482464, 37.035686895251274, 34.89392343908548, 36.87281720340252, 48.228053376078606, 43.71656198054552, 55.28439488261938, 47.59492911398411, 43.14813483506441, 36.02020535618067, 36.087868735194206, 34.40370503813028, 36.18098050355911, 36.5666002035141, 36.0134681686759, 36.25575453042984, 35.68615671247244, 35.83358880132437, 36.40018031001091, 36.41171660274267, 35.984307527542114, 37.35232260078192, 35.58490239083767, 36.29382234066725, 35.9809435904026, 37.03386429697275, 42.08798985928297, 40.878661908209324, 36.050076596438885, 35.22916883230209, 37.95441146939993, 36.1896613612771, 38.27355336397886, 37.52609807997942, 37.64782473444939, 36.41432151198387, 36.07902303338051, 35.90146917849779, 42.206158861517906, 36.5160396322608, 35.90540029108524, 35.11282708495855, 37.925115786492825, 36.260356195271015, 36.768412217497826, 37.84614522010088, 37.21919283270836, 37.078047171235085, 38.37379161268473, 35.5446869507432, 37.346492521464825, 43.91758423298597, 41.149500757455826, 36.10972594469786, 36.08141280710697, 41.63795802742243, 35.93667130917311, 35.53412854671478, 38.23987673968077, 37.22896333783865, 35.404058173298836, 34.746501594781876, 42.12553519755602, 40.91891460120678, 36.33890952914953, 35.126092843711376, 37.460497580468655, 42.000641115009785, 37.783958949148655, 41.57780110836029, 35.64872033894062, 34.478927962481976, 35.97993589937687, 37.41113469004631, 36.11200675368309, 42.487695813179016, 40.78710172325373, 34.90455728024244, 34.08921975642443, 38.3855476975441, 37.86530438810587, 37.10909280925989, 41.66000708937645, 38.356611505150795, 34.81438849121332, 38.61600160598755, 46.379744075238705, 44.59367785602808, 39.873252622783184, 43.34478173404932, 38.20215351879597, 37.88652457296848, 36.4491306245327, 40.645068511366844, 41.536382399499416, 34.599004313349724, 37.21522819250822, 37.88289241492748, 40.56115448474884, 42.013674043118954, 35.31774878501892, 36.725737154483795, 37.30207309126854, 42.201763950288296, 39.722150191664696, 36.94497887045145, 41.44493117928505, 35.51916312426329, 33.80736615508795, 38.300647400319576, 36.44038364291191, 37.00217232108116, 32.92729239910841, 35.730861127376556, 38.87033276259899, 37.62123826891184, 39.68822583556175, 36.547038704156876, 38.01542054861784, 40.02920165657997, 35.09041666984558, 34.011625684797764, 36.1412288621068, 35.435864701867104, 34.74795166403055, 35.33591981977224, 37.62346226722002, 37.72379271686077, 36.18248272687197, 35.474393516778946, 36.74824070185423, 35.35791952162981, 35.54214257746935, 36.443352699279785, 37.67652250826359, 37.480306811630726, 36.768557503819466, 35.323869436979294, 32.42457192391157, 35.0253451615572, 35.167559050023556, 35.82663834095001, 45.01710273325443, 36.133090034127235, 38.43240346759558, 34.871673211455345, 35.67860554903746, 35.00983119010925, 34.40311271697283, 37.41688746958971, 36.73588577657938, 35.63091531395912, 34.66090466827154, 34.87796429544687, 35.04022862762213, 36.10432334244251, 35.32654978334904, 35.97481083124876, 35.90995632112026, 34.567732363939285, 33.08085724711418, 34.57956202328205, 36.44380532205105, 42.19119716435671, 44.72909402102232, 36.91860381513834, 38.4526364505291, 35.85855383425951, 36.293537355959415, 35.764165222644806, 36.049870774149895, 35.11951584368944, 35.99812462925911, 35.509719513356686, 36.05193737894297, 36.936123855412006, 42.20958426594734, 44.86747458577156, 43.18080469965935, 50.168177112936974, 42.75203216820955, 41.71325173228979, 42.50930529087782, 42.3236433416605, 35.15110816806555, 45.88571563363075, 52.8635922819376, 43.275825679302216, 41.179210878908634, 37.820395082235336, 35.42112186551094, 38.06270565837622, 33.71996618807316, 36.7183405905962, 34.53321103006601, 37.02431730926037, 35.60827765613794, 38.528863340616226, 39.6155621856451, 36.23440768569708, 37.81723231077194, 36.157081834971905, 38.65753300487995, 36.65510844439268, 36.672486923635006, 37.271066568791866, 40.30840191990137, 36.55819781124592, 36.485331133008, 36.03851329535246, 36.722853779792786, 36.267656832933426, 37.19937242567539, 36.76897939294577, 43.81019249558449, 39.71715737134218, 38.7380626052618, 35.968516021966934, 35.75513605028391, 36.40429396182299, 39.925835095345974, 45.560671016573906, 38.07099722325802, 41.21948406100273, 44.67024467885494, 35.86220275610685, 36.026548594236374, 35.495974123477936, 35.014997236430645, 36.6998752579093, 36.97092831134796, 38.55851944535971, 37.98259887844324, 40.670255199074745, 36.561518907547, 37.70126774907112, 37.50479593873024, 36.241221241652966, 42.47802961617708, 38.49556017667055, 37.97158598899841, 34.843653440475464, 39.679991081357, 37.118762731552124, 36.25285532325506, 38.09091076254845, 38.472590036690235, 37.50451933592558, 36.37672774493694, 38.38226478546858, 43.46021264791489, 36.80494800209999, 37.62044571340084, 41.056773625314236, 34.46862380951643, 34.555843099951744, 44.48661953210831, 43.36293414235115, 37.401421926915646, 38.37326820939779, 36.61209065467119, 35.267483443021774, 39.76884204894304, 44.52838655561209, 43.92795357853174, 38.13602589070797, 35.48984136432409, 33.78891572356224, 34.397502429783344, 42.19880420714617, 37.73424308747053, 41.49354249238968, 38.60265202820301, 35.907384008169174, 37.05701045691967, 38.136023096740246, 35.90795584022999, 43.506406247615814, 42.924776673316956, 36.37140151113272, 39.57327641546726, 42.69949346780777, 37.36572712659836, 36.43824625760317, 36.71250678598881, 34.98437162488699, 35.8190406113863, 42.16934088617563, 39.042373187839985, 36.3343171775341, 36.917831748723984, 35.938601940870285, 33.68354495614767, 36.38967499136925, 34.673514775931835, 36.54517885297537, 38.13553601503372, 38.881043903529644, 41.80585313588381, 34.55254342406988, 34.79113336652517, 38.10367453843355, 38.11206016689539, 36.478739231824875, 42.13318228721619, 35.93474347144365, 34.708122722804546, 35.45587416738272, 38.66819478571415, 38.91929890960455, 38.516162894666195, 39.853544905781746, 35.34994926303625, 37.31401916593313, 36.69394366443157, 35.1942777633667, 36.86015773564577, 35.48335935920477, 45.118107460439205, 38.315155543386936, 33.563315868377686, 35.707264207303524, 34.57272797822952, 34.498090855777264, 34.076170064508915, 36.015644669532776, 38.56697492301464, 40.704735554754734, 36.204224452376366, 35.53502634167671, 35.20766273140907, 35.71447543799877, 33.94626826047897, 33.93777832388878, 36.042723804712296, 34.88862980157137, 35.124958492815495, 36.165849305689335, 34.40890181809664, 35.11027805507183, 45.16785126179457, 36.1448023468256, 37.83352393656969, 39.99015502631664, 41.994864121079445, 35.71878094226122, 34.80533603578806, 35.57597752660513, 34.75190605968237, 35.19842494279146, 35.106043331325054, 34.85857415944338, 35.22436413913965, 34.42708868533373, 35.01543682068586, 35.651025362312794, 37.10982296615839, 35.83109378814697, 35.41142772883177, 36.66033037006855, 35.75485199689865, 36.53370123356581, 36.727000027894974, 36.01059038192034, 37.20065765082836, 35.127502866089344, 38.388111628592014, 34.94209796190262, 38.210565224289894, 34.50187388807535, 37.344436161220074, 35.99969483911991, 42.01383050531149, 35.97543854266405, 48.180609941482544, 39.67965114861727, 42.12291818112135, 37.69301436841488, 36.31490468978882, 37.0113467797637, 37.50181011855602, 35.74828151613474, 37.23058011382818, 36.85049433261156, 36.0577255487442, 35.67820321768522, 37.67747711390257, 40.54146632552147, 49.341858364641666, 45.31650152057409, 41.940039955079556, 37.32708282768726, 33.02228916436434, 33.1379072740674, 34.76972598582506, 35.36349907517433, 36.73554304987192, 34.791603684425354, 38.873340934515, 36.57647967338562, 33.78316294401884, 39.60094787180424, 44.723182916641235, 37.74874843657017, 37.43669483810663, 41.41614772379398, 35.5973020195961, 35.700815729796886, 36.612655967473984, 36.63450758904219, 40.25120474398136, 41.518472135066986, 37.05971222370863, 47.708901576697826, 42.42660943418741, 42.51300171017647, 44.059090316295624, 39.9760352447629, 35.58722138404846, 33.674041740596294, 36.308533512055874, 41.328541934490204, 36.39250807464123, 35.80924216657877, 37.84284368157387, 36.68106161057949, 36.648291163146496, 38.877710700035095, 44.034344144165516, 37.01559640467167, 38.512563332915306, 38.417077623307705, 33.36303308606148, 38.634827360510826, 56.541997008025646, 47.326709143817425, 53.72532643377781, 45.94821110367775, 44.923619367182255, 39.162496104836464, 34.96422525495291, 34.6111049875617, 33.71327091008425, 37.29632496833801, 38.324966095387936, 35.66508740186691, 36.2448850646615, 36.47005092352629, 37.07318939268589, 37.39634528756142, 36.1820962280035, 35.79279035329819, 38.02698943763971, 42.988634668290615, 36.30969673395157, 38.36097940802574, 35.53343843668699, 37.45428007096052, 40.957421995699406, 36.54536232352257, 34.264287911355495, 38.38677890598774, 34.44964066147804, 35.70176288485527, 38.541958667337894, 37.63814177364111, 35.20176839083433, 35.377467051148415, 38.31890504807234, 36.92004643380642, 38.78161497414112, 42.46901907026768, 39.86304625868797, 34.45391822606325, 33.299860544502735, 36.3378394395113, 36.908313632011414, 36.12110484391451, 37.035271525382996, 41.90133325755596, 34.97286140918732, 38.48498407751322, 37.51457203179598, 35.753666423261166, 36.103020422160625, 36.09167691320181, 38.120148703455925, 41.5026294067502, 37.78277896344662, 42.662207037210464, 35.19865497946739, 38.35673816502094, 37.15725336223841, 38.32803852856159, 40.4224144294858, 35.81058233976364, 39.77752756327391, 37.32176683843136, 36.52571886777878, 34.538513980805874, 35.78640706837177, 33.897921442985535, 35.306221805512905, 38.26426062732935, 36.0086252912879, 38.33067510277033, 46.49083502590656, 36.628879606723785, 38.47509156912565, 33.82931090891361, 38.2741941139102, 35.79770214855671, 36.90453339368105, 35.604494623839855, 36.67019680142403, 34.11005809903145, 36.21603175997734, 34.1549888253212, 35.340373404324055, 34.58461444824934, 36.99782211333513, 34.12456065416336, 34.93470326066017, 32.82763157039881, 33.346484415233135, 34.69706978648901, 34.469105303287506, 33.33504032343626, 34.43769086152315, 35.119786858558655, 33.64897146821022, 34.364739432930946, 33.462043851614, 34.96163059026003, 34.42315571010113, 35.648190416395664, 36.22219059616327, 39.67410326004028, 38.95377181470394, 37.171403877437115, 38.061595521867275, 41.98888223618269, 35.73550935834646, 36.159747280180454, 37.30074409395456, 37.4822998419404, 37.87379991263151, 35.080913454294205, 36.9712021201849, 36.552129313349724, 38.06713689118624, 40.9055994823575, 36.15927044302225, 35.49917135387659, 37.53067273646593, 36.110362969338894, 36.730785854160786, 36.97529900819063, 38.307277485728264, 36.883510649204254, 36.29591595381498, 42.2176830470562, 44.507612474262714, 37.81838994473219, 43.58027037233114, 42.31432359665632, 39.80587422847748, 38.27470541000366, 35.3270685300231, 41.916114278137684, 41.35881643742323, 37.307833321392536, 36.71197593212128, 35.39523761719465, 36.886466667056084, 42.436069808900356, 43.933019042015076, 37.46973443776369, 38.77574857324362, 38.74049615114927, 33.885114826262, 36.22877784073353, 42.23920963704586, 42.93323587626219, 35.8878904953599, 35.83393897861242, 38.49935531616211, 36.543685011565685, 42.17904154211283, 39.70329836010933, 42.45351441204548, 38.361769169569016, 33.82776211947203, 50.98462663590908, 42.79634170234203, 43.13040990382433, 41.97230655699968, 34.28421635180712, 38.15839905291796, 37.232303991913795, 38.80625218153, 42.40254033356905, 35.90590786188841, 35.10879073292017, 36.447031423449516, 42.008460499346256, 39.036741480231285, 36.681657657027245, 34.4787547364831, 39.45461008697748, 42.16213431209326, 37.03756537288427, 37.7001129090786, 42.45069436728954, 35.317132249474525, 36.405942402780056, 38.722725585103035, 36.742876283824444, 40.26490077376366, 41.04230925440788, 36.667163483798504, 35.36367882043123, 41.99013393372297, 35.604823380708694, 34.607721492648125, 42.000328190624714, 41.29687137901783, 36.31329629570246, 36.93051356822252, 37.92090527713299, 38.11539337038994, 38.58361206948757, 42.79807489365339, 40.52905645221472, 42.50882379710674, 35.88946629315615, 38.02180755883455, 41.48314893245697, 34.4872772693634, 36.26369871199131, 41.961981914937496, 35.7055040076375, 35.54160986095667, 36.84941865503788, 38.121819496154785, 41.47372394800186, 47.05432988703251, 47.7472860366106, 55.53633160889149, 53.40931657701731, 49.63031504303217, 47.3431097343564, 42.18874406069517, 37.89726831018925, 41.516706347465515, 35.42126435786486, 37.96620201319456, 34.75802578032017, 37.2790414839983, 37.01633773744106, 36.556572653353214, 37.894073873758316, 38.5314179584384, 45.26010435074568, 39.62087817490101, 42.22465958446264, 35.34153290092945, 36.93341929465532, 37.374009378254414, 36.010767333209515, 37.09064330905676, 35.44139675796032, 37.23385650664568, 36.086576990783215, 34.594304859638214, 34.35968887060881, 36.15352790802717, 34.097207710146904, 39.080494083464146, 34.49287358671427, 45.13799212872982, 44.1350219771266, 37.323436699807644, 37.86906599998474, 35.399858839809895, 35.57714633643627, 37.507456727325916, 36.64223104715347, 37.31814585626125, 34.88586377352476, 36.46381665021181, 36.44788544625044, 35.13011708855629, 36.184968426823616, 35.596626810729504, 35.5874290689826, 34.17561575770378, 36.393978632986546, 35.013312473893166, 35.70289816707373, 36.75141930580139, 37.368472665548325, 38.98943401873112, 34.25249084830284, 37.01396752148867, 36.28958202898502, 37.09976188838482, 35.696420818567276, 36.04947775602341, 37.2037123888731, 37.510085850954056, 37.24424168467522, 35.221424885094166, 36.077079363167286, 36.68023366481066, 37.24538628011942, 42.552029713988304, 36.45776864141226, 36.88144963234663, 33.24317652732134, 34.864635206758976, 35.53754463791847, 33.877236768603325, 35.02112627029419, 35.78750602900982, 33.02528150379658, 33.25227554887533, 32.58065972477198, 34.70522537827492, 35.10016668587923, 36.6105642169714, 33.239214681088924, 37.08052076399326, 45.935879461467266, 34.82808079570532, 36.296370439231396, 34.273325465619564, 34.482283517718315, 33.951135352253914, 40.05480371415615, 47.20620717853308, 37.40029502660036, 38.82164042443037, 44.03170384466648, 44.17669400572777, 37.27484308183193, 36.5376528352499, 36.15105431526899, 35.67991405725479, 35.773622803390026, 38.253466598689556, 35.83395853638649, 36.75369918346405, 36.498394794762135, 36.88764851540327, 36.31256986409426, 36.234292201697826, 62.72721104323864, 53.11244446784258, 62.48678546398878, 54.15188707411289, 41.58908128738403, 45.339930802583694, 38.18601183593273, 33.813894726336, 35.33652983605862, 45.10482773184776, 38.071501068770885, 33.68932008743286, 36.34040616452694, 34.761528484523296, 42.05465968698263, 35.45719850808382, 37.29265555739403, 38.19040209054947, 38.04129175841808, 37.02363092452288, 35.49684397876263, 37.187119014561176, 39.38975092023611, 38.860080763697624, 36.117324605584145, 33.27090386301279, 35.21811496466398, 44.367700815200806, 34.008908085525036, 42.078050784766674, 36.29632014781237, 35.99546477198601, 33.61410927027464, 37.61440888047218, 34.626878798007965, 42.07094106823206, 40.809644386172295, 35.73267348110676, 42.69507713615894, 34.63280852884054, 33.28079916536808, 34.813255071640015, 34.860413521528244, 34.50369369238615, 32.00053051114082, 36.225948482751846, 33.24695862829685, 37.229121662676334, 36.41729522496462, 37.525939755141735, 41.225118562579155, 41.54904745519161, 45.12631148099899, 39.56253547221422, 42.26095601916313, 36.802965216338634, 31.742382794618607, 43.75795181840658, 34.94247514754534, 35.79907212406397, 38.14804647117853, 35.88197473436594, 34.71606597304344, 34.95014272630215, 42.25079994648695, 36.60011012107134, 37.616061978042126, 37.01533377170563, 41.2540128454566, 42.27575659751892, 32.53615740686655, 35.40653083473444, 38.464752957224846, 37.90475055575371, 36.28516383469105, 42.04278625547886, 48.962317407131195, 42.493049055337906, 42.334762401878834, 36.99428495019674, 34.51129328459501, 36.83881461620331, 34.96189322322607, 36.18265315890312, 44.46671903133392, 41.10389109700918, 37.04666718840599, 36.57580725848675, 36.28676291555166, 33.84728450328112, 35.48251651227474, 42.79063083231449, 41.52939189225435, 36.55211627483368, 35.32915934920311, 34.93345994502306, 38.48214354366064, 36.78113128989935, 36.929160356521606, 34.62816774845123, 38.931580260396004, 40.56455101817846, 35.79966817051172, 34.91351008415222, 34.558399580419064, 34.34768691658974, 38.54562155902386, 38.30556757748127, 36.81421559303999, 36.76423616707325, 38.59602473676205, 36.33078932762146, 35.570849664509296, 35.96722800284624, 37.62072790414095, 36.96402441710234, 37.3627794906497, 37.75020968168974, 43.71599853038788, 38.12043834477663, 38.819548673927784, 35.04026681184769, 34.72802322357893, 36.934022791683674, 37.42728661745787, 37.46878821402788, 36.879836581647396, 34.99681409448385, 35.238584503531456, 34.83928367495537, 37.8956301137805, 41.24966636300087, 43.658629059791565, 39.80934154242277, 39.975667372345924, 38.16458862274885, 37.46249061077833, 35.40925029665232, 36.034890450537205, 37.48645633459091, 35.427192226052284, 33.188583329319954, 33.741915598511696, 35.92244163155556, 34.69408396631479, 34.18745473027229, 35.75334884226322, 38.753786124289036, 38.52225374430418, 37.578980438411236, 45.64246628433466, 36.82208713144064, 39.73441943526268, 34.29372049868107, 38.25271409004927, 34.59588997066021, 38.999306969344616, 34.758297726511955, 36.74573544412851, 34.187182784080505, 37.42579836398363, 34.1402143239975, 37.12579607963562, 36.191307939589024, 38.002862595021725, 34.61025562137365, 34.43377837538719, 34.07352138310671, 37.524509243667126, 34.22437980771065, 35.774849355220795, 34.45393592119217, 35.5394771322608, 34.00282096117735, 35.43840814381838, 34.38041638582945, 36.20546218007803, 34.72473379224539, 35.20971164107323, 35.08313000202179, 35.80438159406185, 35.576376132667065, 35.36540828645229, 35.34456808120012, 37.370054982602596, 35.92024743556976, 36.63776163011789, 35.82518268376589, 38.17531932145357, 35.700248554348946, 36.4761408418417, 35.82985419780016, 41.31835885345936, 35.63902247697115, 38.06975297629833, 40.710956789553165, 35.82102805376053, 35.608201287686825, 38.18375989794731, 38.09644002467394, 36.12983040511608, 35.30037682503462, 38.561745546758175, 37.82099951058626, 36.65238432586193, 36.276211962103844, 36.656053736805916, 36.9363771751523, 38.811867125332355, 42.460826225578785, 41.3482915610075, 36.891959607601166, 35.76998878270388, 37.709484808146954, 35.02350207418203, 36.24153509736061, 37.225174717605114, 37.30585053563118, 37.22583036869764, 37.727560847997665, 38.09330891817808, 36.111422814428806, 35.08298844099045, 36.279684863984585, 37.99720387905836, 38.78669999539852, 44.90098636597395, 35.56734882295132, 36.253456957638264, 37.376715801656246, 42.38763730973005, 43.02367381751537, 34.81</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mu (qps)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cv</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t># requests</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Latency Constraint (ms)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Planner</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estimated Latency (ms)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Ingest mu Observed (qps)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Throughput (qps)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>p95 (ms)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>p99 (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>SimulatedAnnealing</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>71.74977540969849</v>
+      </c>
+      <c r="H2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="J2" t="n">
+        <v>98.7417827834613</v>
+      </c>
+      <c r="K2" t="n">
+        <v>247.5048317183545</v>
+      </c>
+      <c r="L2" t="n">
+        <v>44.5681876502931</v>
+      </c>
+      <c r="M2" t="n">
+        <v>54.17011484503745</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mu (qps)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cv</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t># requests</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Latency Constraint (ms)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Planner</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estimated Latency (ms)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Latency (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>SimulatedAnnealing</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>71.74977540969849</v>
+      </c>
+      <c r="H2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>[66.28575269132853, 49.01054874062538, 58.38960316032171, 76.3660753145814, 80.79917170107365, 88.46969995647669, 83.77821277827024, 79.18474450707436, 69.09528374671936, 65.33174868673086, 56.172505021095276, 52.532169967889786, 42.32942871749401, 35.89181322604418, 36.62949614226818, 37.83306200057268, 36.304702050983906, 42.76850074529648, 40.18335975706577, 42.28022322058678, 38.29693701118231, 38.20497449487448, 37.01616730540991, 40.30816350132227, 42.50824637711048, 38.76840230077505, 38.943005725741386, 43.353174813091755, 39.394501596689224, 36.507981829345226, 38.6157613247633, 39.009276777505875, 40.091692470014095, 37.92570158839226, 36.81995812803507, 54.052979685366154, 44.086046516895294, 49.10940770059824, 44.49135810136795, 42.92425513267517, 36.35224141180515, 34.26032606512308, 37.12906502187252, 42.200665920972824, 37.24395390599966, 35.094691440463066, 40.664201602339745, 35.6884254142642, 36.344108171761036, 42.94456262141466, 42.06747282296419, 36.833553574979305, 35.486229695379734, 36.13172098994255, 38.12618926167488, 39.21688813716173, 35.254865884780884, 38.71949203312397, 42.90460515767336, 36.63042560219765, 39.78273086249828, 41.52592923492193, 36.08180861920118, 38.27584907412529, 43.82144659757614, 35.77713668346405, 36.38288192451, 42.384108528494835, 44.91701629012823, 36.721027456223965, 37.673414684832096, 41.96296166628599, 34.894571639597416, 39.29680958390236, 44.838021509349346, 35.78408341854811, 36.26142721623182, 43.964783661067486, 35.29506269842386, 34.81970448046923, 35.87490972131491, 36.63903474807739, 36.7627190425992, 34.866683185100555, 38.54539431631565, 39.764244109392166, 36.77928075194359, 39.73742574453354, 38.69061451405287, 40.81382602453232, 36.279876716434956, 35.98837461322546, 38.11250161379576, 35.48619896173477, 35.98640486598015, 36.96842771023512, 39.7775424644351, 35.5919050052762, 37.20912802964449, 37.98883408308029, 37.14332822710276, 36.8075966835022, 35.021327435970306, 37.67387196421623, 38.00593409687281, 35.98362673074007, 43.41044556349516, 52.52836551517248, 42.0411117374897, 44.28511671721935, 37.94929478317499, 36.31547838449478, 34.70178134739399, 36.1968781799078, 38.544063456356525, 44.93189603090286, 47.1882913261652, 37.639787420630455, 39.92816433310509, 36.266147159039974, 42.40712895989418, 43.811025097966194, 38.99105731397867, 41.9948548078537, 35.28760187327862, 37.82312851399183, 35.32437980175018, 36.32346913218498, 35.13358533382416, 37.36191801726818, 34.706137143075466, 35.30460316687822, 37.42429334670305, 36.118676885962486, 35.99955793470144, 38.016196340322495, 38.5092468932271, 34.33302789926529, 35.38079746067524, 37.256418727338314, 34.780303947627544, 36.7325060069561, 35.680041648447514, 37.188672460615635, 34.5141151919961, 36.39253415167332, 35.00268142670393, 36.34136449545622, 36.026906222105026, 36.149715073406696, 36.21903993189335, 36.34964954108, 35.52806843072176, 37.51329332590103, 35.64383648335934, 38.31454925239086, 35.87204311043024, 37.74596843868494, 34.583997912704945, 36.95081267505884, 35.110765136778355, 36.1391780897975, 51.91092099994421, 43.08398626744747, 36.940754391252995, 36.72618791460991, 34.83026381582022, 38.38017489761114, 34.93120800703764, 37.305775098502636, 35.03197617828846, 39.368982426822186, 34.86586548388004, 42.31045115739107, 38.648320361971855, 47.02089540660381, 38.24524115771055, 40.744989179074764, 45.10397929698229, 38.06820418685675, 38.22010010480881, 43.510984629392624, 36.35289520025253, 35.85759550333023, 36.84768360108137, 38.03517296910286, 38.426198065280914, 36.03083919733763, 38.94611541181803, 38.348219357430935, 37.64111269265413, 38.81849627941847, 44.99304573982954, 37.69153542816639, 38.65435998886824, 42.41515509784222, 35.534621216356754, 35.90725641697645, 37.54967451095581, 43.51726267486811, 37.91389148682356, 37.486009299755096, 36.726776510477066, 37.720258347690105, 39.34304881840944, 46.19651101529598, 55.29715120792389, 47.79167752712965, 49.35302585363388, 44.42225489765406, 41.58437065780163, 34.77609995752573, 39.583662524819374, 41.8776273727417, 42.14003775268793, 56.08836933970451, 45.814490877091885, 46.744316816329956, 55.68780843168497, 56.68863281607628, 52.434454672038555, 52.869378589093685, 42.61157847940922, 42.76559501886368, 35.775271244347095, 35.960244946181774, 43.112222105264664, 44.55346893519163, 36.36498190462589, 36.3645926117897, 37.299529649317265, 36.839564330875874, 38.54909632354975, 42.69709158688784, 43.34981832653284, 37.62286342680454, 35.62485706061125, 40.31871818006039, 37.17769496142864, 36.67317796498537, 42.36946627497673, 40.17381276935339, 37.8904240205884, 38.11343293637037, 43.3428268879652, 40.7789871096611, 38.78321498632431, 43.28239895403385, 43.132321909070015, 49.108450300991535, 42.421686463057995, 41.64711758494377, 33.550444059073925, 43.32854971289635, 42.45411418378353, 41.662235744297504, 36.216397769749165, 33.8414441794157, 34.85302533954382, 37.64962963759899, 35.49569100141525, 37.31277771294117, 38.840681314468384, 34.605203196406364, 37.059709429740906, 37.46071644127369, 34.95626989752054, 37.838016636669636, 37.59108390659094, 35.66211648285389, 35.578894428908825, 38.89940865337849, 36.705038510262966, 33.01320597529411, 33.192877657711506, 33.267322927713394, 42.39192046225071, 35.906716249883175, 34.04704108834267, 37.930408492684364, 36.909691989421844, 35.35204008221626, 33.767797984182835, 36.29050310701132, 37.489461712539196, 34.654672257602215, 35.22863611578941, 36.213223822414875, 35.9520148485899, 37.96317148953676, 36.06259636580944, 34.77275837212801, 35.49772035330534, 35.91123875230551, 34.57257803529501, 36.67572606354952, 34.9004752933979, 35.89098900556564, 36.83868981897831, 34.77947786450386, 38.487608544528484, 36.0517418012023, 36.16679273545742, 35.14106757938862, 34.805613569915295, 34.42126978188753, 35.42754240334034, 35.22734623402357, 33.88151898980141, 34.91361252963543, 35.8069334179163, 40.06194695830345, 43.58064942061901, 36.556294187903404, 36.14279069006443, 37.579745054244995, 35.331024788320065, 35.494981333613396, 36.223593167960644, 35.28078831732273, 42.13234595954418, 46.12443782389164, 51.70831177383661, 42.86997392773628, 43.26185770332813, 37.39147633314133, 33.914826810359955, 38.460809737443924, 33.33003260195255, 38.17019797861576, 35.14482919126749, 41.121567599475384, 34.80949625372887, 36.768737249076366, 33.904033713042736, 37.215521559119225, 34.68353487551212, 46.27275001257658, 43.7288461253047, 48.20846579968929, 38.46075665205717, 36.336641758680344, 36.29374038428068, 34.14386883378029, 35.36137938499451, 36.56052425503731, 37.66235243529081, 41.80096834897995, 33.98487064987421, 34.92665197700262, 32.19166584312916, 35.54070554673672, 35.12469865381718, 37.97176945954561, 36.5587305277586, 41.35463200509548, 37.4843068420887, 37.07566298544407, 37.498876452445984, 37.67654858529568, 37.28813584893942, 36.84817720204592, 39.97431788593531, 36.67989559471607, 34.74984224885702, 36.38762701302767, 36.22672241181135, 36.429909989237785, 36.5343252196908, 38.031780160963535, 41.0895561799407, 35.27768328785896, 35.935621708631516, 36.00735682994127, 38.22935372591019, 37.960502319037914, 39.495743811130524, 35.89130938053131, 34.42012704908848, 36.14204563200474, 41.090852580964565, 35.602199845016, 34.00189522653818, 34.16551370173693, 32.94764179736376, 32.004572451114655, 33.5180489346385, 34.157159738242626, 35.23837309330702, 42.33748372644186, 42.24460106343031, 35.5640621855855, 34.858111292123795, 44.00114435702562, 36.570088006556034, 35.85982695221901, 35.05482152104378, 40.792147628962994, 33.733353950083256, 34.93828233331442, 36.56828589737415, 38.165765814483166, 36.402844823896885, 35.60759034007788, 39.756408892571926, 38.27922698110342, 35.280187614262104, 40.320100262761116, 43.64587087184191, 37.42162324488163, 37.19855099916458, 42.996994219720364, 34.32987630367279, 34.558056853711605, 41.05086252093315, 43.84277667850256, 35.96766106784344, 35.31964495778084, 40.75501672923565, 38.33483345806599, 33.37402734905481, 34.258910454809666, 37.92477957904339, 40.42914602905512, 34.38608720898628, 38.2736437022686, 33.76699611544609, 36.264754831790924, 36.556681618094444, 35.21289024502039, 38.85935340076685, 37.0200565084815, 37.69587352871895, 36.24093625694513, 36.52120567858219, 37.76231687515974, 33.912185579538345, 37.16729395091534, 38.00624515861273, 40.468065068125725, 34.68347992748022, 38.47073391079903, 42.5812928006053, 36.88790276646614, 35.09490378201008, 36.38427797704935, 33.977605402469635, 34.91123113781214, 35.006800666451454, 36.950831301510334, 36.33832838386297, 37.332918494939804, 35.80749686807394, 35.099128261208534, 36.595496349036694, 35.95568984746933, 34.71851907670498, 36.211663857102394, 35.41389852762222, 35.88796965777874, 36.88152972608805, 34.708816558122635, 34.71768833696842, 37.164260633289814, 36.94016207009554, 37.2154600918293, 34.982907585799694, 34.91742163896561, 34.79783236980438, 34.982701763510704, 35.35815142095089, 34.79331452399492, 37.045298144221306, 35.66319029778242, 34.240687265992165, 36.5517009049654, 34.40740145742893, 36.18829697370529, 34.38675031065941, 35.647764801979065, 34.00031756609678, 37.89162915199995, 33.97552389651537, 33.313567750155926, 37.74679638445377, 39.234863594174385, 44.14561949670315, 37.292794324457645, 37.419602274894714, 37.27514296770096, 36.414594389498234, 37.392305210232735, 35.31191311776638, 41.703629307448864, 35.58297082781792, 36.05247754603624, 35.03958694636822, 35.463424399495125, 34.81628559529781, 35.941957496106625, 34.47937872260809, 35.6746269389987, 34.483847208321095, 35.33310815691948, 33.95209368318319, 35.82448698580265, 34.6213998273015, 36.86534985899925, 36.38644050806761, 38.40097784996033, 36.53402253985405, 35.76596174389124, 37.40137070417404, 35.71662586182356, 35.15291120857, 36.53625212609768, 35.036505199968815, 35.79001873731613, 33.56847167015076, 34.767698496580124, 34.7095150500536, 34.8492581397295, 35.711342468857765, 36.21276095509529, 38.02559059113264, 34.855837002396584, 34.41821411252022, 33.830481581389904, 33.618586137890816, 33.97782705724239, 37.76030894368887, 37.17865515500307, 34.66314449906349, 34.81902275234461, 35.907791927456856, 34.86790228635073, 34.61109846830368, 35.44866759330034, 36.241001449525356, 35.20165663212538, 35.543221049010754, 33.963936381042004, 35.17967741936445, 33.74477755278349, 34.79448705911636, 35.217964090406895, 34.26607605069876, 35.24860925972462, 33.880291506648064, 34.037431702017784, 33.67026522755623, 33.747417852282524, 34.226568415760994, 33.8300708681345, 34.313793294131756, 34.519584849476814, 34.120758064091206, 33.98329671472311, 33.989910036325455, 33.941417932510376, 41.34134016931057, 36.05653904378414, 35.51448881626129, 43.94597839564085, 41.60525184124708, 45.98847031593323, 37.83819731324911, 35.749378614127636, 36.35633736848831, 33.0581059679389, 35.36162152886391, 34.40261259675026, 35.63099354505539, 34.44633260369301, 35.75675282627344, 35.44002119451761, 36.12341918051243, 35.970221273601055, 36.19478829205036, 35.955714993178844, 36.85024566948414, 36.68764140456915, 37.92322054505348, 38.45690842717886, 46.90349940210581, 37.78791055083275, 42.05760546028614, 40.542454458773136, 40.448921732604504, 36.65473498404026, 35.36595031619072, 41.19709134101868, 38.18714153021574, 36.476217210292816, 36.55377496033907, 38.52619789540768, 36.70071251690388, 37.66209818422794, 39.14507478475571, 37.90923301130533, 36.727153696119785, 37.40090411156416, 37.4805573374033, 37.29799576103687, 35.20053345710039, 35.4215782135725, 37.77940105646849, 44.34073809534311, 43.603675439953804, 38.71970158070326, 42.781357653439045, 36.04183066636324, 33.22399780154228, 37.34896145761013, 35.5193093419075, 37.901220843195915, 42.250228114426136, 38.784004747867584, 40.6129565089941, 53.55121288448572, 43.83103083819151, 44.18800212442875, 41.20715893805027, 36.03168576955795, 36.999630741775036, 37.23295498639345, 34.8511328920722, 35.802421160042286, 37.75269165635109, 44.39534805715084, 40.87329562753439, 36.01010609418154, 34.524304792284966, 36.903792060911655, 38.69359474629164, 37.80053462833166, 37.47312258929014, 36.44179459661245, 34.52967666089535, 39.14382494986057, 38.693721406161785, 37.603420205414295, 35.22688243538141, 41.999259032309055, 37.57447563111782, 36.8237653747201, 34.47297494858503, 38.40330708771944, 40.063487365841866, 34.79450661689043, 34.990101121366024, 42.01218765228987, 40.693280287086964, 35.83961818367243, 34.9286450073123, 38.55327609926462, 38.19906525313854, 37.41686325520277, 38.54420967400074, 36.65955737233162, 37.09740936756134, 34.872270189225674, 35.75011156499386, 39.077614434063435, 38.66806998848915, 37.68197447061539, 37.78245486319065, 36.261532455682755, 36.09263617545366, 34.714408218860626, 36.878105252981186, 41.76966194063425, 43.94662473350763, 52.48308088630438, 43.009805493056774, 44.18603517115116, 39.72166869789362, 35.501995123922825, 37.589230574667454, 36.33616864681244, 40.71181174367666, 36.67388204485178, 40.89922457933426, 35.65997909754515, 34.74408574402332, 36.36403754353523, 36.187415942549706, 36.19558364152908, 33.76071434468031, 35.93418840318918, 36.060928367078304, 33.384804613888264, 36.51112783700228, 35.96732672303915, 35.98430100828409, 35.30232887715101, 38.05041033774614, 40.079216472804546, 34.643872641026974, 36.21294070035219, 35.28225235641003, 36.77681088447571, 34.55027937889099, 36.51140816509724, 37.009626626968384, 42.53599140793085, 35.04152316600084, 38.83795719593763, 35.12940276414156, 36.34142130613327, 35.88204924017191, 35.546441562473774, 34.74090062081814, 35.575841553509235, 33.880398608744144, 43.69399417191744, 38.642775267362595, 37.414563819766045, 38.106922060251236, 37.111965008080006, 32.84195996820927, 35.81587318331003, 34.440853632986546, 35.536497831344604, 36.96370869874954, 38.26138284057379, 34.098134376108646, 36.979387514293194, 34.84201617538929, 38.89608010649681, 34.63471960276365, 38.79240155220032, 34.082941710948944, 37.390271201729774, 34.961000084877014, 37.36214525997639, 34.816126339137554, 38.88722788542509, 35.328155383467674, 37.9333421587944, 37.670886144042015, 41.12892970442772, 38.41258119791746, 45.843265019357204, 48.603457398712635, 39.19909801334143, 44.313233345746994, 38.377899676561356, 34.405190497636795, 37.28100378066301, 34.3239177018404, 37.37530671060085, 36.66521701961756, 37.51096222549677, 37.99057379364967, 37.90052607655525, 36.96595039218664, 42.47222561389208, 38.58216945081949, 34.132528118789196, 38.07164076715708, 35.806866362690926, 38.42868749052286, 37.668801844120026, 45.05026340484619, 42.011795565485954, 53.490664809942245, 46.76445107907057, 56.25895783305168, 63.54724895209074, 53.83611284196377, 47.19557520002127, 44.340251944959164, 43.33274997770786, 36.17624845355749, 36.92764602601528, 34.026394598186016, 34.326501190662384, 38.44214044511318, 41.47586226463318, 36.16728167980909, 37.51273825764656, 37.57684584707022, 36.13703045994043, 52.75510810315609, 43.28468628227711, 45.380531810224056, 43.316518887877464, 36.57148405909538, 35.3726539760828, 35.34819185733795, 34.809877164661884, 40.23793525993824, 41.646855883300304, 42.38426219671965, 41.8000565841794, 38.23601733893156, 34.83600355684757, 38.045614026486874, 36.06751002371311, 37.041942588984966, 42.40285139530897, 37.394434213638306, 37.90706489235163, 38.59551623463631, 37.77533024549484, 45.27186416089535, 40.519509464502335, 37.94122580438852, 42.127303779125214, 35.996150225400925, 36.55966557562351, 33.3261089399457, 35.31500976532698, 43.30790042877197, 43.41262485831976, 36.08566801995039, 35.60813516378403, 34.69184506684542, 35.26837658137083, 37.52639517188072, 35.69585271179676, 34.275006502866745, 33.468821085989475, 38.11576496809721, 37.94380836188793, 35.51274351775646, 36.61559522151947, 36.81320417672396, 44.59945112466812, 36.06963250786066, 37.47532609850168, 36.79458424448967, 32.415393739938736, 40.93771707266569, 39.62970431894064, 35.45728325843811, 37.61165775358677, 36.829449236392975, 35.43767333030701, 34.26620364189148, 37.77922410517931, 37.45393734425306, 34.46117229759693, 35.28066910803318, 37.08379715681076, 38.688257336616516, 36.110603250563145, 37.98964526504278, 36.83908376842737, 35.296727903187275, 34.02021247893572, 34.93777569383383, 35.84648668766022, 36.23410128057003, 36.87661327421665, 36.950940266251564, 34.15971901267767, 35.37776693701744, 36.31352912634611, 34.48291588574648, 34.54067651182413, 38.116793148219585, 36.51144914329052, 36.167534068226814, 36.02081071585417, 35.76550167053938, 35.913124680519104, 36.226315423846245, 35.90995725244284, 34.091465175151825, 34.88927986472845, 35.85403971374035, 37.14374266564846, 37.66700346022844, 41.29743669182062, 34.36574432998896, 37.91532572358847, 35.74042487889528, 34.32779852300882, 35.16196832060814, 35.373165272176266, 35.798775032162666, 35.53916793316603, 34.986251033842564, 35.29668226838112, 34.95970740914345, 34.856983460485935, 34.15275923907757, 35.027080215513706, 36.14513576030731, 45.113932341337204, 36.86290420591831, 36.769009195268154, 37.97017503529787, 35.25021579116583, 42.129382491111755, 35.642134957015514, 41.69132933020592, 35.5465030297637, 37.75253985077143, 36.935131065547466, 39.68519996851683, 36.902603693306446, 38.46864774823189, 41.3886709138751, 52.09933500736952, 43.409417383372784, 46.76785599440336, 39.47908524423838, 37.2672937810421, 36.687024869024754, 38.58956415206194, 45.89561279863119, 36.92894894629717, 38.77976071089506, 35.24999972432852, 36.775472573935986, 35.93365475535393, 36.68771032243967, 36.12740524113178, 37.97936253249645, 36.51953302323818, 38.66994194686413, 38.313036784529686, 38.15283067524433, 35.97643040120602, 34.79057736694813, 36.34228091686964, 35.148789174854755, 32.44390990585089, 35.05945764482021, 35.04182677716017, 37.37450856715441, 36.35172639042139, 38.06876949965954, 37.72090468555689, 38.23274001479149, 36.45458538085222, 38.144996389746666, 42.46573708951473, 37.63360343873501, 36.52795497328043, 45.01868970692158, 36.71874571591616, 40.436520241200924, 38.65404054522514, 37.01137751340866, 36.509172059595585, 41.492316871881485, 36.308121867477894, 36.315588280558586, 42.46973805129528, 41.17748141288757, 36.32504492998123, 36.913877353072166, 45.55681813508272, 35.94328463077545, 39.0866557136178, 42.29503311216831, 35.82512028515339, 35.90891882777214, 41.97682160884142, 37.94550150632858, 36.650086753070354, 35.44546104967594, 43.854027055203915, 41.48340970277786, 37.222870625555515, 35.309646278619766, 40.06259422749281, 41.75218939781189, 33.690908923745155, 34.55776534974575, 34.43933371454477, 36.54039464890957, 36.262379959225655, 43.28609351068735, 41.23445972800255, 35.7037428766489, 35.045936703681946, 42.5831088796258, 42.117489501833916, 36.1047750338912, 39.06103689223528, 38.419648073613644, 36.2459197640419, 36.102413199841976, 43.34457591176033, 37.57119178771973, 36.7662962526083, 38.4866027161479, 42.001708410680294, 39.939855225384235, 36.44517343491316, 34.483836963772774, 38.64336106926203, 43.11615414917469, 37.32043504714966, 37.567662075161934, 38.01602777093649, 37.86551021039486, 37.40313369780779, 43.42262540012598, 41.48935340344906, 35.86902562528849, 36.06310859322548, 34.711241722106934, 37.4347772449255, 42.18823183327913, 40.366931818425655, 35.23617424070835, 33.86652283370495, 45.805285684764385, 37.264506332576275, 37.88878954946995, 37.08008490502834, 32.492668367922306, 34.66828726232052, 38.45628350973129, 42.49172750860453, 44.39575131982565, 37.4300442636013, 35.03489959985018, 37.746334448456764, 40.36806523799896, 34.05665513128042, 33.55175442993641, 42.789991945028305, 36.98373772203922, 35.62611248344183, 37.17995714396238, 36.932678893208504, 36.85281239449978, 33.65716338157654, 36.27845644950867, 38.50278630852699, 37.438017316162586, 36.113206297159195, 37.074027583003044, 37.975178100168705, 38.77898212522268, 35.55962257087231, 36.53283230960369, 36.57326102256775, 37.04031091183424, 35.9619315713644, 34.89803895354271, 37.52007149159908, 37.116050720214844, 34.09989923238754, 37.50511538237333, 36.63642331957817, 34.91224907338619, 35.75330041348934, 38.927734829485416, 39.764225482940674, 41.75411909818649, 36.15306504070759, 38.050953298807144, 35.466295666992664, 37.814946845173836, 34.59276631474495, 36.57035809010267, 36.457362584769726, 37.01647464185953, 38.31721097230911, 39.69347383826971, 34.590951167047024, 36.94318886846304, 33.4544125944376, 43.47129072993994, 35.92928033322096, 38.25673088431358, 37.0668163523078, 37.6931531354785, 36.644977517426014, 35.382227040827274, 36.27417888492346, 34.598096273839474, 35.37412825971842, 35.039011389017105, 36.35120391845703, 39.430840872228146, 40.793364867568016, 36.30915563553572, 38.460247218608856, 35.98474711179733, 37.50878665596247, 35.76981741935015, 37.486555986106396, 36.27779521048069, 36.75930295139551, 37.19318564981222, 36.30727529525757, 36.933695897459984, 38.844335824251175, 36.607371643185616, 36.102594807744026, 36.476398818194866, 41.384369134902954, 41.33253823965788, 40.85494112223387, 50.89017190039158, 42.221032083034515, 42.625452391803265, 56.39120005071163, 45.933240093290806, 52.635181695222855, 48.39649237692356, 44.12901494652033, 43.0294880643487, 35.122900269925594, 35.25401744991541, 34.42197199910879, 34.68200471252203, 36.104632541537285, 37.98751439899206, 34.741515293717384, 35.81481799483299, 35.79441457986832, 37.05690614879131, 34.59283709526062, 37.49105613678694, 34.83046405017376, 37.616899237036705, 34.66784209012985, 37.80870698392391, 35.115672275424004, 33.971537835896015, 42.448692955076694, 42.304023168981075, 36.74800135195255, 35.51219683140516, 37.71307598799467, 35.262566059827805, 36.17631737142801, 35.878753289580345, 33.31743739545345, 32.69088175147772, 32.49584883451462, 32.08117559552193, 33.05014967918396, 36.98466531932354, 35.57322267442942, 43.126973323524, 38.62523473799229, 41.37224704027176, 36.05274297297001, 33.20486471056938, 36.84728126972914, 35.61726026237011, 37.60728985071182, 36.379922181367874, 36.58990003168583, 36.218466237187386, 42.353213764727116, 36.32403910160065, 37.17928659170866, 36.09684016555548, 43.5531921684742, 40.707836858928204, 36.9062926620245, 35.79624369740486, 37.81572077423334, 35.902407951653004, 36.22053284198046, 38.18721417337656, 39.193724282085896, 35.84578353911638, 35.930247977375984, 38.437530398368835, 34.242493100464344, 37.815903313457966, 36.15600802004337, 38.378285244107246, 35.90322658419609, 40.24989623576403, 43.21398679167032, 36.843789741396904, 37.13992144912481, 44.96543575078249, 36.16776317358017, 38.53403031826019, 38.6837562546134, 33.50182995200157, 35.76582111418247, 38.90185710042715, 37.807054817676544, 36.50742117315531, 37.989155389368534, 42.033630423247814, 42.06009954214096, 37.932454608380795, 40.96193239092827, 34.40630529075861, 34.66514125466347, 40.32374173402786, 36.66329011321068, 38.974275812506676, 38.315299898386, 43.642500415444374, 38.50078396499157, 37.53789979964495, 37.393417209386826, 33.57805125415325, 38.279879838228226, 39.160105399787426, 38.74051570892334, 44.64167356491089, 37.8690967336297, 35.93714069575071, 36.5075645968318, 33.00292696803808, 38.67317829281092, 42.36036166548729, 41.699339635670185, 33.58612023293972, 33.00397377461195, 32.231906428933144, 35.23636609315872, 35.35897471010685, 38.17808721214533, 42.000578716397285, 36.09545063227415, 37.01282013207674, 35.37233825773001, 32.70001523196697, 37.206687964499, 37.83744014799595, 37.03221492469311, 37.51697484403849, 36.00879851728678, 35.18306463956833, 36.927453242242336, 35.5329317972064, 41.45961347967386, 41.06968641281128, 34.4831133261323, 39.92562275379896, 35.12896038591862, 33.0096734687686, 36.6573603823781, 38.05700037628412, 37.69764956086874, 36.80285066366196, 34.307921305298805, 34.51265022158623, 37.054781801998615, 36.561496555805206, 40.000107139348984, 38.37849199771881, 43.09265315532684, 36.23639885336161, 38.628553971648216, 35.50366126000881, 34.100499004125595, 35.4157742112875, 33.65670423954725, 38.166651502251625, 35.64839344471693, 36.57808434218168, 36.44712641835213, 35.56029684841633, 35.732473246753216, 35.80132964998484, 35.56566871702671, 37.726069800555706, 38.06945402175188, 35.24560481309891, 38.11379335820675, 48.57197031378746, 35.51098611205816, 42.00265184044838, 34.5771387219429, 42.96069871634245, 35.312945023179054, 37.53169160336256, 35.310763865709305, 37.40666154772043, 34.95929203927517, 37.23225649446249, 38.02288789302111, 42.41983965039253, 35.196248441934586, 37.11198270320892, 35.45279894024134, 37.90311794728041, 35.88978946208954, 38.45537640154362, 38.079009391367435, 36.68344859033823, 35.08050739765167, 36.948748864233494, 34.550595097243786, 37.754678167402744, 36.56602464616299, 38.48448675125837, 36.675737239420414, 42.959293350577354, 37.03621402382851, 34.58571992814541, 38.651986978948116, 33.7299220263958, 38.21753244847059, 34.547063522040844, 37.45618183165789, 35.87284032255411, 36.87982261180878, 37.81295567750931, 36.735073663294315, 36.603196524083614, 38.03405072540045, 34.080496057868004, 38.71886618435383, 35.70947144180536, 38.91421388834715, 43.32826752215624, 36.946192383766174, 38.40878698974848, 42.304390110075474, 35.017295740544796, 36.44356597214937, 36.566306836903095, 42.466492392122746, 37.099373526871204, 37.13022265583277, 47.9368232190609, 41.72928165644407, 42.85853635519743, 35.86295712739229, 33.64988323301077, 37.97760512679815, 35.638040862977505, 42.281326837837696, 38.235691376030445, 59.58624929189682, 54.156335070729256, 63.707184977829456, 54.84532378613949, 46.04693595319986, 44.95037253946066, 35.70038639008999, 48.30407723784447, 34.549095667898655, 36.77284810692072, 35.67096311599016, 37.75347862392664, 39.78927340358496, 36.96873690932989, 36.338478326797485, 35.946217365562916, 42.552159167826176, 40.524786338210106, 35.54229252040386, 34.446206875145435, 41.90247040241957, 36.8163101375103, 35.366286523640156, 35.83239670842886, 36.90508008003235, 37.91463375091553, 37.51359414309263, 36.336627788841724, 36.68978903442621, 37.24443353712559, 40.05735740065575, 43.709006160497665, 41.2305174395442, 37.85979375243187, 34.147423692047596, 38.27693685889244, 38.15075475722551, 34.92189850658178, 36.97854373604059, 43.587551452219486, 36.94888483732939, 41.28275252878666, 36.70661523938179, 36.540063098073006, 37.94609569013119, 44.58092898130417, 38.475388661026955, 35.87053157389164, 44.342185370624065, 34.71345454454422, 35.90805642306805, 44.88895647227764, 36.32909897714853, 40.04307463765144, 36.280171014368534, 36.95040941238403, 36.68105788528919, 37.52955049276352, 37.65225224196911, 35.99936701357365, 38.666910491883755, 41.89248010516167, 36.49322222918272, 35.75076628476381, 45.55497970432043, 36.03585250675678, 36.0931446775794, 34.526037983596325, 38.88229560106993, 40.3030039742589, 37.40214463323355, 35.62934324145317, 46.486638486385345, 34.586356952786446, 43.34663599729538, 34.66050047427416, 43.824346736073494, 45.11130973696709, 40.41755385696888, 42.02759079635143, 32.46046602725983, 39.95492961257696, 35.15750542283058, 35.26353742927313, 35.579838789999485, 35.31842399388552, 36.850620061159134, 36.52427904307842, 37.579234689474106, 38.44782430678606, 37.93046250939369, 35.209319554269314, 35.33147368580103, 34.629546105861664, 38.329798728227615, 38.061169907450676, 37.10614889860153, 38.770562037825584, 39.71924539655447, 42.51199308782816, 41.620341129601, 38.58346585184336, 37.20420133322477, 36.57830134034157, 34.795355051755905, 36.640701815485954, 35.58680787682533, 36.79507412016392, 38.51575870066881, 34.766195341944695, 37.58453205227852, 41.62850696593523, 35.06794013082981, 37.90875617414713, 38.996447809040546, 37.9706546664238, 40.20229447633028, 34.985640086233616, 38.278683088719845, 37.21318393945694, 37.23905794322491, 36.73647716641426, 37.6084940508008, 36.554502323269844, 35.68309638649225, 36.089799366891384, 35.56712716817856, 36.195230670273304, 35.636793822050095, 35.85417848080397, 36.676046438515186, 38.64995948970318, 39.74674269556999, 35.44216323643923, 36.9182787835598, 36.24940011650324, 36.08872648328543, 36.0686844214797, 35.83529870957136, 35.03517899662256, 35.63075605779886, 35.12566536664963, 35.25933809578419, 35.11768952012062, 34.50469020754099, 35.629063844680786, 34.76841468364, 35.89897230267525, 34.62623059749603, 39.55909051001072, 41.47878661751747, 34.13716610521078, 35.329654812812805, 36.31629701703787, 34.325688146054745, 37.44693752378225, 34.1821676120162, 39.40196242183447, 34.21257343143225, 43.511075899004936, 35.3837963193655, 42.065633460879326, 38.09687774628401, 41.89374577254057, 41.177645325660706, 37.665482610464096, 36.994386464357376, 37.681302055716515, 38.10455556958914, 33.21904316544533, 35.170464776456356, 34.108009189367294, 42.13300999253988, 41.80879518389702, 34.109869971871376, 35.201434046030045, 36.286620423197746, 35.34368332475424, 36.847904324531555, 40.081472136080265, 38.03313057869673, 47.41236660629511, 38.95848151296377, 34.453012980520725, 44.72262132912874, 32.76892099529505, 43.870837427675724, 34.36579927802086, 43.692595325410366, 38.155741058290005, 46.675209887325764, 37.601834163069725, 42.3330357298255, 35.700143314898014, 34.77694187313318, 42.402319610118866, 36.25843487679958, 37.25750558078289, 38.752119056880474, 37.61198092252016, 38.098826073110104, 34.170402213931084, 35.82594636827707, 37.86620311439037, 42.88919735699892, 36.296517588198185, 37.48409729450941, 38.000679574906826, 37.43840008974075, 36.681889556348324, 36.98041383177042, 35.95631290227175, 38.26427273452282, 41.02305695414543, 36.393774673342705, 34.91103835403919, 43.08760724961758, 37.44401689618826, 38.41059282422066, 35.49976833164692, 37.78663091361523, 38.14102616161108, 36.54076438397169, 38.18441368639469, 38.475526496768, 39.35880772769451, 38.429287262260914, 44.622077606618404, 44.400524348020554, 41.84047784656286, 36.60288453102112, 35.18431633710861, 35.764665342867374, 34.32478476315737, 33.955877646803856, 38.28583378344774, 37.10215538740158, 37.6337468624115, 39.94066175073385, 35.807203501462936, 38.69012277573347, 41.46559536457062, 37.0068559423089, 38.40353526175022, 41.84683412313461, 38.017033599317074, 38.19844499230385, 39.185237139463425, 35.0583316758275, 32.59514458477497, 36.833097226917744, 36.190633662045, 42.33803320676088, 37.6688651740551, 35.77486891299486, 35.6623874977231, 41.67287424206734, 36.07737272977829, 33.06138329207897, 37.76837233453989, 43.391128070652485, 34.340741112828255, 34.334215335547924, 40.54637439548969, 36.11074388027191, 38.5782765224576, 33.57865661382675, 33.82177837193012, 40.17867334187031, 43.36579795926809, 42.68332105129957, 44.56211533397436, 38.81682828068733, 41.43098276108503, 35.451692529022694, 35.82244273275137, 36.96858696639538, 35.37062369287014, 35.83178389817476, 33.026447519659996, 35.849922336637974, 40.081510320305824, 35.88254936039448, 37.530056200921535, 35.609726794064045, 36.65843326598406, 34.43458303809166, 33.12141168862581, 35.62177158892155, 36.737323738634586, 33.8076576590538, 35.47234367579222, 36.98670398443937, 38.796151988208294, 42.08550602197647, 36.20643727481365, 38.03474362939596, 35.772922448813915, 34.76430382579565, 34.81129743158817, 34.98451877385378, 34.20558758080006, 35.917168483138084, 37.54173591732979, 34.99079402536154, 34.995028749108315, 33.87628588825464, 35.427107475697994, 34.1242291033268, 36.25458665192127, 37.010300904512405, 35.60073394328356, 38.26395235955715, 45.655316673219204, 37.9058588296175, 38.058691658079624, 33.585598692297935, 35.013786517083645, 33.0289751291275, 35.4735404253006, 34.062257036566734, 35.39882320910692, 34.370278008282185, 35.64871661365032, 34.37902592122555, 35.05172673612833, 36.15038190037012, 38.7137271463871, 35.338892601430416, 37.27981634438038, 36.3049004226923, 35.90611554682255, 36.024970933794975, 37.377817556262016, 35.73369234800339, 37.011394277215004, 36.79355140775442, 41.61731339991093, 41.951789520680904, 34.89039186388254, 35.628536716103554, 35.79736314713955, 35.94585973769426, 39.099941961467266, 38.473524153232574, 38.835770450532436, 36.596424877643585, 32.7352425083518, 37.41018660366535, 32.805779948830605, 35.4603435844183, 35.580286756157875, 37.95600030571222, 38.753475062549114, 33.30318070948124, 33.61862991005182, 32.51743409782648, 35.76313517987728, 36.241025663912296, 36.441413685679436, 42.832011356949806, 37.11844328790903, 35.99154110997915, 35.871827974915504, 34.45693664252758, 38.25470432639122, 36.04776877909899, 44.938371516764164, 42.725</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mu (qps)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cv</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t># requests</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Latency Constraint (ms)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Planner</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estimated Latency (ms)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Ingest mu Observed (qps)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Throughput (qps)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>p95 (ms)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>p99 (ms)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>100</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>SimulatedAnnealing</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>71.74977540969849</v>
+      </c>
+      <c r="H2" t="n">
+        <v>22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>75.8</v>
+      </c>
+      <c r="J2" t="n">
+        <v>98.72362501810282</v>
+      </c>
+      <c r="K2" t="n">
+        <v>243.3695312986856</v>
+      </c>
+      <c r="L2" t="n">
+        <v>48.41661527752873</v>
+      </c>
+      <c r="M2" t="n">
+        <v>130.6685947999358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>